<commit_message>
04: Updated graphs, exponential fit
</commit_message>
<xml_diff>
--- a/04_RozpadPlazmatu/data/Rozpadgrafy.xlsx
+++ b/04_RozpadPlazmatu/data/Rozpadgrafy.xlsx
@@ -15,9 +15,44 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>y0</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>R0</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Exponential</t>
+  </si>
+  <si>
+    <t>Equation</t>
+  </si>
+  <si>
+    <t>y = y0 + A*exp(R0*x)</t>
+  </si>
+  <si>
+    <t>Plot</t>
+  </si>
+  <si>
+    <t>1/n</t>
+  </si>
+  <si>
+    <t>Odchylka</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -26,16 +61,29 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -43,11 +91,87 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -65,6 +189,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,15 +512,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE16"/>
+  <dimension ref="A1:AE26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="8.88671875" style="14"/>
+    <col min="1" max="2" width="8.88671875" style="14"/>
+    <col min="3" max="3" width="10.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.3">
@@ -1497,6 +1645,191 @@
       <c r="G16" s="4">
         <v>13.446595827758761</v>
       </c>
+    </row>
+    <row r="18" spans="2:27" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="B18" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:27" ht="34.200000000000003" x14ac:dyDescent="0.3">
+      <c r="B19" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B20" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B21" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="24">
+        <f>-0.000000381</f>
+        <v>-3.8099999999999998E-7</v>
+      </c>
+      <c r="D21" s="23">
+        <v>1.39E-8</v>
+      </c>
+      <c r="F21" s="23">
+        <v>-3.6899999999999998E-7</v>
+      </c>
+      <c r="G21" s="23">
+        <v>5.2399999999999999E-8</v>
+      </c>
+      <c r="J21" s="23">
+        <v>-2.4200000000000002E-7</v>
+      </c>
+      <c r="K21" s="23">
+        <v>2.9000000000000002E-8</v>
+      </c>
+      <c r="N21" s="23">
+        <v>-6.8099999999999994E-8</v>
+      </c>
+      <c r="O21" s="23">
+        <v>1.85E-8</v>
+      </c>
+      <c r="R21" s="23">
+        <v>-1.29E-8</v>
+      </c>
+      <c r="S21" s="23">
+        <v>3.2299999999999998E-9</v>
+      </c>
+      <c r="V21" s="23">
+        <v>-4.9199999999999997E-8</v>
+      </c>
+      <c r="W21" s="23">
+        <v>8.9899999999999998E-9</v>
+      </c>
+      <c r="Z21" s="23">
+        <v>-2.9799999999999999E-7</v>
+      </c>
+      <c r="AA21" s="23">
+        <v>6.6600000000000001E-8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B22" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="24">
+        <f>0.000000419</f>
+        <v>4.1899999999999998E-7</v>
+      </c>
+      <c r="D22" s="23">
+        <f>0.0000000118</f>
+        <v>1.18E-8</v>
+      </c>
+      <c r="F22" s="23">
+        <v>4.1100000000000001E-7</v>
+      </c>
+      <c r="G22" s="23">
+        <v>4.7799999999999998E-8</v>
+      </c>
+      <c r="J22" s="23">
+        <v>2.6600000000000003E-7</v>
+      </c>
+      <c r="K22" s="23">
+        <v>2.59E-8</v>
+      </c>
+      <c r="N22" s="23">
+        <v>8.2399999999999997E-8</v>
+      </c>
+      <c r="O22" s="23">
+        <v>1.26E-8</v>
+      </c>
+      <c r="R22" s="23">
+        <v>4.1099999999999997E-8</v>
+      </c>
+      <c r="S22" s="23">
+        <v>2.3499999999999999E-9</v>
+      </c>
+      <c r="V22" s="23">
+        <v>7.4200000000000003E-8</v>
+      </c>
+      <c r="W22" s="23">
+        <v>6.7999999999999997E-9</v>
+      </c>
+      <c r="Z22" s="23">
+        <v>3.0800000000000001E-7</v>
+      </c>
+      <c r="AA22" s="23">
+        <v>6.1900000000000005E-8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B23" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="24">
+        <f>0.00203</f>
+        <v>2.0300000000000001E-3</v>
+      </c>
+      <c r="D23" s="23">
+        <f>0.0000289</f>
+        <v>2.8900000000000001E-5</v>
+      </c>
+      <c r="F23" s="23">
+        <v>1.56E-3</v>
+      </c>
+      <c r="G23" s="23">
+        <v>1.05E-4</v>
+      </c>
+      <c r="J23" s="23">
+        <v>1.8E-3</v>
+      </c>
+      <c r="K23" s="23">
+        <v>9.48E-5</v>
+      </c>
+      <c r="N23" s="23">
+        <v>2.65E-3</v>
+      </c>
+      <c r="O23" s="23">
+        <v>1.5799999999999999E-4</v>
+      </c>
+      <c r="R23" s="23">
+        <v>2.2599999999999999E-3</v>
+      </c>
+      <c r="S23" s="23">
+        <v>5.4599999999999999E-5</v>
+      </c>
+      <c r="V23" s="23">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="W23" s="23">
+        <v>4.88E-5</v>
+      </c>
+      <c r="Z23" s="23">
+        <v>3.97E-4</v>
+      </c>
+      <c r="AA23" s="23">
+        <v>5.0899999999999997E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B24" s="19"/>
+      <c r="C24" s="20"/>
+    </row>
+    <row r="25" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B25" s="19"/>
+      <c r="C25" s="20"/>
+    </row>
+    <row r="26" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B26" s="21"/>
+      <c r="C26" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
04: Corrected Dodělat grafy
</commit_message>
<xml_diff>
--- a/04_RozpadPlazmatu/data/Rozpadgrafy.xlsx
+++ b/04_RozpadPlazmatu/data/Rozpadgrafy.xlsx
@@ -1,17 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\Škola Mgr\Praktikum plazma\PraktikaPlazma\04_RozpadPlazmatu\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0E92BA-DB52-4EA4-B96E-1D00439784DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="108" windowWidth="19140" windowHeight="10872"/>
+    <workbookView xWindow="345" yWindow="570" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -126,12 +144,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.0E+00"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0E+00"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -302,19 +320,19 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -322,12 +340,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -369,7 +390,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -402,9 +423,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -437,6 +475,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -612,18 +667,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
@@ -633,48 +688,70 @@
     <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="22">
+        <f>5*1.59</f>
+        <v>7.95</v>
+      </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
       <c r="E1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="22"/>
+      <c r="F1" s="22">
+        <f>10*1.59</f>
+        <v>15.9</v>
+      </c>
       <c r="G1" s="22"/>
       <c r="H1" s="22"/>
       <c r="I1" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="22"/>
+      <c r="J1" s="22">
+        <f>20*1.59</f>
+        <v>31.8</v>
+      </c>
       <c r="K1" s="22"/>
       <c r="L1" s="22"/>
       <c r="M1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="22"/>
+      <c r="N1" s="22">
+        <f>50*1.59</f>
+        <v>79.5</v>
+      </c>
       <c r="O1" s="22"/>
       <c r="P1" s="22"/>
       <c r="Q1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="22"/>
+      <c r="R1" s="22">
+        <f>100*1.59</f>
+        <v>159</v>
+      </c>
       <c r="S1" s="22"/>
       <c r="T1" s="22"/>
       <c r="U1" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="22"/>
+      <c r="V1" s="22">
+        <f>200*1.59</f>
+        <v>318</v>
+      </c>
       <c r="W1" s="22"/>
       <c r="X1" s="22"/>
       <c r="Y1" s="22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="Z1">
+        <f>450*1.59</f>
+        <v>715.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>43</v>
       </c>
@@ -732,14 +809,14 @@
       <c r="Y2" s="11">
         <v>280</v>
       </c>
-      <c r="Z2" s="12">
-        <v>4.6055300414299055E-8</v>
+      <c r="Z2" s="19">
+        <v>4.6055300414299102E-8</v>
       </c>
       <c r="AA2" s="12">
         <v>16.893422979581029</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>50</v>
       </c>
@@ -804,7 +881,7 @@
         <v>16.81159498480773</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>60</v>
       </c>
@@ -869,7 +946,7 @@
         <v>16.766692438187018</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>74</v>
       </c>
@@ -934,7 +1011,7 @@
         <v>16.604609143634047</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>92</v>
       </c>
@@ -999,7 +1076,7 @@
         <v>16.470978194037965</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>115</v>
       </c>
@@ -1064,7 +1141,7 @@
         <v>16.366104307158352</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>144</v>
       </c>
@@ -1129,7 +1206,7 @@
         <v>16.170873601587623</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>190</v>
       </c>
@@ -1194,7 +1271,7 @@
         <v>15.952423320705165</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>248</v>
       </c>
@@ -1259,7 +1336,7 @@
         <v>15.658254255367595</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>324</v>
       </c>
@@ -1324,7 +1401,7 @@
         <v>15.406426743442815</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>416</v>
       </c>
@@ -1389,7 +1466,7 @@
         <v>15.182127790498003</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>500</v>
       </c>
@@ -1454,7 +1531,7 @@
         <v>14.995171231199933</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>600</v>
       </c>
@@ -1519,7 +1596,7 @@
         <v>14.673227095141588</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>700</v>
       </c>
@@ -1584,7 +1661,7 @@
         <v>14.611249394865721</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>800</v>
       </c>
@@ -1649,7 +1726,7 @@
         <v>14.500474989363804</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>3</v>
       </c>
@@ -1660,7 +1737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="34.200000000000003" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" ht="24" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>5</v>
       </c>
@@ -1668,7 +1745,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>7</v>
       </c>
@@ -1682,7 +1759,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>0</v>
       </c>
@@ -1733,7 +1810,7 @@
         <v>6.6600000000000001E-8</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>1</v>
       </c>
@@ -1785,7 +1862,7 @@
         <v>6.1900000000000005E-8</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>2</v>
       </c>
@@ -1837,7 +1914,7 @@
         <v>5.0899999999999997E-5</v>
       </c>
     </row>
-    <row r="24" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
         <v>27</v>
       </c>
@@ -1898,7 +1975,7 @@
         <v>50.9</v>
       </c>
     </row>
-    <row r="25" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>24</v>
       </c>
@@ -1960,7 +2037,7 @@
         <v>3.3899399999999998E-6</v>
       </c>
     </row>
-    <row r="26" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>25</v>
       </c>
@@ -2021,11 +2098,11 @@
         <v>7.1280812237153196E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B27" s="14"/>
       <c r="E27" s="14"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B28" s="22" t="s">
         <v>8</v>
       </c>
@@ -2033,7 +2110,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>12</v>
       </c>
@@ -2080,7 +2157,7 @@
         <v>8.4700000000000007E-9</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
         <v>13</v>
       </c>
@@ -2127,7 +2204,7 @@
         <v>6.5799999999999998E-12</v>
       </c>
     </row>
-    <row r="31" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
         <v>26</v>
       </c>
@@ -2188,7 +2265,7 @@
         <v>6.5799999999999997E-6</v>
       </c>
     </row>
-    <row r="32" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
         <v>24</v>
       </c>
@@ -2250,7 +2327,7 @@
         <v>6.5799999999999997E-6</v>
       </c>
     </row>
-    <row r="33" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
@@ -2268,7 +2345,7 @@
       <c r="Z33" s="19"/>
       <c r="AA33" s="19"/>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B34" s="22" t="s">
         <v>14</v>
       </c>
@@ -2277,7 +2354,7 @@
       </c>
       <c r="D34" s="19"/>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
         <v>12</v>
       </c>
@@ -2325,7 +2402,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
         <v>13</v>
       </c>
@@ -2373,7 +2450,7 @@
         <v>5.7500000000000002E-5</v>
       </c>
     </row>
-    <row r="37" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>26</v>
       </c>
@@ -2435,7 +2512,7 @@
         <v>57.5</v>
       </c>
     </row>
-    <row r="38" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
         <v>25</v>
       </c>
@@ -2497,10 +2574,10 @@
         <v>8.0523510876941238E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="D39" s="19"/>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
         <v>15</v>
       </c>
@@ -2510,7 +2587,7 @@
       </c>
       <c r="D40" s="19"/>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
         <v>23</v>
       </c>
@@ -2520,49 +2597,49 @@
       </c>
       <c r="D41" s="19"/>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="D42" s="19"/>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="D43" s="19"/>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="29" t="s">
+      <c r="B44" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C44" s="29"/>
-      <c r="D44" s="30" t="s">
+      <c r="C44" s="33"/>
+      <c r="D44" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="E44" s="30"/>
-      <c r="F44" s="29" t="s">
+      <c r="E44" s="34"/>
+      <c r="F44" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="33"/>
       <c r="J44" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="K44" s="29" t="s">
+      <c r="K44" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="L44" s="29"/>
-      <c r="M44" s="30" t="s">
+      <c r="L44" s="33"/>
+      <c r="M44" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="N44" s="30"/>
-      <c r="O44" s="29" t="s">
+      <c r="N44" s="34"/>
+      <c r="O44" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="P44" s="29"/>
-      <c r="Q44" s="29"/>
-      <c r="R44" s="29"/>
-    </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="P44" s="33"/>
+      <c r="Q44" s="33"/>
+      <c r="R44" s="33"/>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B45" s="12" t="s">
         <v>24</v>
       </c>
@@ -2615,7 +2692,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <v>5</v>
       </c>
@@ -2623,7 +2700,7 @@
         <f>B32</f>
         <v>2.0100000000000001E-3</v>
       </c>
-      <c r="C46" s="31">
+      <c r="C46" s="29">
         <f>C32</f>
         <v>1.1399999999999999E-4</v>
       </c>
@@ -2631,7 +2708,7 @@
         <f>B38</f>
         <v>5.7276723388989502E-2</v>
       </c>
-      <c r="E46" s="31">
+      <c r="E46" s="29">
         <f>C38</f>
         <v>2.7588055030882477E-3</v>
       </c>
@@ -2639,7 +2716,7 @@
         <f>B25</f>
         <v>7.7343000000000008E-4</v>
       </c>
-      <c r="G46" s="31">
+      <c r="G46" s="29">
         <f>C25</f>
         <v>4.0171000000000002E-7</v>
       </c>
@@ -2647,47 +2724,47 @@
         <f>B26</f>
         <v>2.84283003617723E-2</v>
       </c>
-      <c r="I46" s="31">
+      <c r="I46" s="29">
         <f>C26</f>
         <v>4.0471816771193075E-4</v>
       </c>
       <c r="J46" s="14">
         <v>5</v>
       </c>
-      <c r="K46" s="32">
-        <f>B46*1000</f>
+      <c r="K46" s="30">
+        <f t="shared" ref="K46:R46" si="0">B46*1000</f>
         <v>2.0100000000000002</v>
       </c>
-      <c r="L46" s="32">
-        <f>C46*1000</f>
+      <c r="L46" s="30">
+        <f t="shared" si="0"/>
         <v>0.11399999999999999</v>
       </c>
-      <c r="M46" s="34">
-        <f>D46*1000</f>
+      <c r="M46" s="32">
+        <f t="shared" si="0"/>
         <v>57.276723388989502</v>
       </c>
-      <c r="N46" s="34">
-        <f>E46*1000</f>
+      <c r="N46" s="32">
+        <f t="shared" si="0"/>
         <v>2.7588055030882477</v>
       </c>
       <c r="O46" s="25">
-        <f>F46*1000</f>
+        <f t="shared" si="0"/>
         <v>0.77343000000000006</v>
       </c>
       <c r="P46" s="25">
-        <f>G46*1000</f>
+        <f t="shared" si="0"/>
         <v>4.0171E-4</v>
       </c>
-      <c r="Q46" s="34">
-        <f>H46*1000</f>
+      <c r="Q46" s="32">
+        <f t="shared" si="0"/>
         <v>28.428300361772301</v>
       </c>
-      <c r="R46" s="34">
-        <f>I46*1000</f>
+      <c r="R46" s="32">
+        <f t="shared" si="0"/>
         <v>0.40471816771193075</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <v>10</v>
       </c>
@@ -2695,7 +2772,7 @@
         <f>F32</f>
         <v>1.2099999999999999E-3</v>
       </c>
-      <c r="C47" s="31">
+      <c r="C47" s="29">
         <f>G32</f>
         <v>5.2199999999999995E-5</v>
       </c>
@@ -2703,7 +2780,7 @@
         <f>F38</f>
         <v>5.0694801630352566E-2</v>
       </c>
-      <c r="E47" s="31">
+      <c r="E47" s="29">
         <f>G38</f>
         <v>3.3049649681666316E-3</v>
       </c>
@@ -2711,7 +2788,7 @@
         <f>F25</f>
         <v>5.7563999999999998E-4</v>
       </c>
-      <c r="G47" s="31">
+      <c r="G47" s="29">
         <f>G25</f>
         <v>5.502E-6</v>
       </c>
@@ -2719,47 +2796,47 @@
         <f>F26</f>
         <v>2.1846378603135361E-2</v>
       </c>
-      <c r="I47" s="31">
+      <c r="I47" s="29">
         <f>G26</f>
         <v>1.4704293290571878E-3</v>
       </c>
       <c r="J47" s="14">
         <v>10</v>
       </c>
-      <c r="K47" s="32">
-        <f t="shared" ref="K47:L52" si="0">B47*1000</f>
+      <c r="K47" s="30">
+        <f t="shared" ref="K47:L52" si="1">B47*1000</f>
         <v>1.21</v>
       </c>
-      <c r="L47" s="32">
-        <f t="shared" si="0"/>
+      <c r="L47" s="30">
+        <f t="shared" si="1"/>
         <v>5.2199999999999996E-2</v>
       </c>
-      <c r="M47" s="34">
-        <f t="shared" ref="M47:M52" si="1">D47*1000</f>
+      <c r="M47" s="32">
+        <f t="shared" ref="M47:M52" si="2">D47*1000</f>
         <v>50.694801630352565</v>
       </c>
-      <c r="N47" s="34">
-        <f t="shared" ref="N47:N52" si="2">E47*1000</f>
+      <c r="N47" s="32">
+        <f t="shared" ref="N47:N52" si="3">E47*1000</f>
         <v>3.3049649681666318</v>
       </c>
-      <c r="O47" s="33">
-        <f t="shared" ref="O47:O52" si="3">F47*1000</f>
+      <c r="O47" s="31">
+        <f t="shared" ref="O47:O52" si="4">F47*1000</f>
         <v>0.57563999999999993</v>
       </c>
-      <c r="P47" s="33">
-        <f t="shared" ref="P47:P52" si="4">G47*1000</f>
+      <c r="P47" s="31">
+        <f t="shared" ref="P47:P52" si="5">G47*1000</f>
         <v>5.5019999999999999E-3</v>
       </c>
-      <c r="Q47" s="34">
-        <f t="shared" ref="Q47:Q52" si="5">H47*1000</f>
+      <c r="Q47" s="32">
+        <f t="shared" ref="Q47:Q52" si="6">H47*1000</f>
         <v>21.84637860313536</v>
       </c>
-      <c r="R47" s="34">
-        <f t="shared" ref="R47:R52" si="6">I47*1000</f>
+      <c r="R47" s="32">
+        <f t="shared" ref="R47:R52" si="7">I47*1000</f>
         <v>1.4704293290571879</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <v>20</v>
       </c>
@@ -2767,7 +2844,7 @@
         <f>J32</f>
         <v>1E-3</v>
       </c>
-      <c r="C48" s="31">
+      <c r="C48" s="29">
         <f>K32</f>
         <v>5.66E-5</v>
       </c>
@@ -2775,7 +2852,7 @@
         <f>J38</f>
         <v>5.6856600723544599E-2</v>
       </c>
-      <c r="E48" s="31">
+      <c r="E48" s="29">
         <f>K38</f>
         <v>2.7307973253919201E-3</v>
       </c>
@@ -2783,7 +2860,7 @@
         <f>J25</f>
         <v>4.3560000000000002E-4</v>
       </c>
-      <c r="G48" s="31">
+      <c r="G48" s="29">
         <f>K25</f>
         <v>2.7491999999999999E-6</v>
       </c>
@@ -2791,47 +2868,47 @@
         <f>J26</f>
         <v>2.5207359926694647E-2</v>
       </c>
-      <c r="I48" s="31">
+      <c r="I48" s="29">
         <f>K26</f>
         <v>1.327587622805918E-3</v>
       </c>
       <c r="J48" s="14">
         <v>20</v>
       </c>
-      <c r="K48" s="32">
-        <f t="shared" si="0"/>
+      <c r="K48" s="30">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L48" s="32">
-        <f t="shared" si="0"/>
+      <c r="L48" s="30">
+        <f t="shared" si="1"/>
         <v>5.6599999999999998E-2</v>
       </c>
-      <c r="M48" s="34">
-        <f t="shared" si="1"/>
+      <c r="M48" s="32">
+        <f t="shared" si="2"/>
         <v>56.856600723544602</v>
       </c>
-      <c r="N48" s="34">
-        <f t="shared" si="2"/>
+      <c r="N48" s="32">
+        <f t="shared" si="3"/>
         <v>2.73079732539192</v>
       </c>
-      <c r="O48" s="33">
-        <f t="shared" si="3"/>
+      <c r="O48" s="31">
+        <f t="shared" si="4"/>
         <v>0.43560000000000004</v>
       </c>
-      <c r="P48" s="33">
-        <f t="shared" si="4"/>
+      <c r="P48" s="31">
+        <f t="shared" si="5"/>
         <v>2.7491999999999998E-3</v>
       </c>
-      <c r="Q48" s="34">
-        <f t="shared" si="5"/>
+      <c r="Q48" s="32">
+        <f t="shared" si="6"/>
         <v>25.207359926694647</v>
       </c>
-      <c r="R48" s="34">
-        <f t="shared" si="6"/>
+      <c r="R48" s="32">
+        <f t="shared" si="7"/>
         <v>1.327587622805918</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <v>50</v>
       </c>
@@ -2839,7 +2916,7 @@
         <f>N32</f>
         <v>8.2199999999999992E-4</v>
       </c>
-      <c r="C49" s="31">
+      <c r="C49" s="29">
         <f>O32</f>
         <v>7.0099999999999996E-5</v>
       </c>
@@ -2847,7 +2924,7 @@
         <f>N38</f>
         <v>5.2655374069095484E-2</v>
       </c>
-      <c r="E49" s="31">
+      <c r="E49" s="29">
         <f>O38</f>
         <v>9.7748540160182574E-4</v>
       </c>
@@ -2855,7 +2932,7 @@
         <f>N25</f>
         <v>1.8046499999999999E-4</v>
       </c>
-      <c r="G49" s="31">
+      <c r="G49" s="29">
         <f>O25</f>
         <v>2.9230000000000002E-6</v>
       </c>
@@ -2863,47 +2940,47 @@
         <f>N26</f>
         <v>3.7110835447633786E-2</v>
       </c>
-      <c r="I49" s="31">
+      <c r="I49" s="29">
         <f>O26</f>
         <v>2.2126460380098635E-3</v>
       </c>
       <c r="J49" s="14">
         <v>50</v>
       </c>
-      <c r="K49" s="32">
-        <f t="shared" si="0"/>
+      <c r="K49" s="30">
+        <f t="shared" si="1"/>
         <v>0.82199999999999995</v>
       </c>
-      <c r="L49" s="32">
-        <f t="shared" si="0"/>
+      <c r="L49" s="30">
+        <f t="shared" si="1"/>
         <v>7.0099999999999996E-2</v>
       </c>
-      <c r="M49" s="34">
-        <f t="shared" si="1"/>
+      <c r="M49" s="32">
+        <f t="shared" si="2"/>
         <v>52.655374069095487</v>
       </c>
-      <c r="N49" s="34">
-        <f t="shared" si="2"/>
+      <c r="N49" s="32">
+        <f t="shared" si="3"/>
         <v>0.97748540160182573</v>
       </c>
-      <c r="O49" s="33">
-        <f t="shared" si="3"/>
+      <c r="O49" s="31">
+        <f t="shared" si="4"/>
         <v>0.18046499999999999</v>
       </c>
-      <c r="P49" s="33">
-        <f t="shared" si="4"/>
+      <c r="P49" s="31">
+        <f t="shared" si="5"/>
         <v>2.9230000000000003E-3</v>
       </c>
-      <c r="Q49" s="34">
-        <f t="shared" si="5"/>
+      <c r="Q49" s="32">
+        <f t="shared" si="6"/>
         <v>37.110835447633789</v>
       </c>
-      <c r="R49" s="34">
-        <f t="shared" si="6"/>
+      <c r="R49" s="32">
+        <f t="shared" si="7"/>
         <v>2.2126460380098636</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="12">
         <v>100</v>
       </c>
@@ -2911,7 +2988,7 @@
         <f>R32</f>
         <v>3.0299999999999999E-4</v>
       </c>
-      <c r="C50" s="31">
+      <c r="C50" s="29">
         <f>S32</f>
         <v>2.0999999999999999E-5</v>
       </c>
@@ -2919,7 +2996,7 @@
         <f>R38</f>
         <v>3.6130549228262331E-2</v>
       </c>
-      <c r="E50" s="31">
+      <c r="E50" s="29">
         <f>S38</f>
         <v>4.5793370533495282E-4</v>
       </c>
@@ -2927,7 +3004,7 @@
         <f>R25</f>
         <v>2.9153999999999999E-5</v>
       </c>
-      <c r="G50" s="31">
+      <c r="G50" s="29">
         <f>S25</f>
         <v>1.76358E-7</v>
       </c>
@@ -2935,47 +3012,47 @@
         <f>R26</f>
         <v>3.1649240796849949E-2</v>
       </c>
-      <c r="I50" s="31">
+      <c r="I50" s="29">
         <f>S26</f>
         <v>7.6462325110973769E-4</v>
       </c>
       <c r="J50" s="14">
         <v>100</v>
       </c>
-      <c r="K50" s="32">
-        <f t="shared" si="0"/>
+      <c r="K50" s="30">
+        <f t="shared" si="1"/>
         <v>0.30299999999999999</v>
       </c>
-      <c r="L50" s="32">
-        <f t="shared" si="0"/>
+      <c r="L50" s="30">
+        <f t="shared" si="1"/>
         <v>2.0999999999999998E-2</v>
       </c>
-      <c r="M50" s="34">
-        <f t="shared" si="1"/>
+      <c r="M50" s="32">
+        <f t="shared" si="2"/>
         <v>36.130549228262332</v>
       </c>
-      <c r="N50" s="34">
-        <f t="shared" si="2"/>
+      <c r="N50" s="32">
+        <f t="shared" si="3"/>
         <v>0.45793370533495281</v>
       </c>
       <c r="O50" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.9153999999999999E-2</v>
       </c>
       <c r="P50" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.7635799999999999E-4</v>
       </c>
-      <c r="Q50" s="34">
-        <f t="shared" si="5"/>
+      <c r="Q50" s="32">
+        <f t="shared" si="6"/>
         <v>31.649240796849949</v>
       </c>
-      <c r="R50" s="34">
-        <f t="shared" si="6"/>
+      <c r="R50" s="32">
+        <f t="shared" si="7"/>
         <v>0.76462325110973772</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="12">
         <v>200</v>
       </c>
@@ -2983,7 +3060,7 @@
         <f>V32</f>
         <v>2.7399999999999999E-4</v>
       </c>
-      <c r="C51" s="31">
+      <c r="C51" s="29">
         <f>W32</f>
         <v>1.5800000000000001E-5</v>
       </c>
@@ -2991,7 +3068,7 @@
         <f>V38</f>
         <v>2.3246787487951729E-2</v>
       </c>
-      <c r="E51" s="31">
+      <c r="E51" s="29">
         <f>W38</f>
         <v>5.8957214050769154E-4</v>
       </c>
@@ -2999,7 +3076,7 @@
         <f>V25</f>
         <v>5.9039999999999997E-5</v>
       </c>
-      <c r="G51" s="31">
+      <c r="G51" s="29">
         <f>W25</f>
         <v>4.3871199999999994E-7</v>
       </c>
@@ -3007,47 +3084,47 @@
         <f>V26</f>
         <v>1.680490661779643E-2</v>
       </c>
-      <c r="I51" s="31">
+      <c r="I51" s="29">
         <f>W26</f>
         <v>6.8339953579038819E-4</v>
       </c>
       <c r="J51" s="14">
         <v>200</v>
       </c>
-      <c r="K51" s="32">
-        <f t="shared" si="0"/>
+      <c r="K51" s="30">
+        <f t="shared" si="1"/>
         <v>0.27399999999999997</v>
       </c>
-      <c r="L51" s="32">
-        <f t="shared" si="0"/>
+      <c r="L51" s="30">
+        <f t="shared" si="1"/>
         <v>1.5800000000000002E-2</v>
       </c>
-      <c r="M51" s="34">
-        <f t="shared" si="1"/>
+      <c r="M51" s="32">
+        <f t="shared" si="2"/>
         <v>23.246787487951728</v>
       </c>
-      <c r="N51" s="34">
-        <f t="shared" si="2"/>
+      <c r="N51" s="32">
+        <f t="shared" si="3"/>
         <v>0.58957214050769158</v>
       </c>
       <c r="O51" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.9039999999999995E-2</v>
       </c>
       <c r="P51" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.3871199999999996E-4</v>
       </c>
-      <c r="Q51" s="34">
-        <f t="shared" si="5"/>
+      <c r="Q51" s="32">
+        <f t="shared" si="6"/>
         <v>16.80490661779643</v>
       </c>
-      <c r="R51" s="34">
-        <f t="shared" si="6"/>
+      <c r="R51" s="32">
+        <f t="shared" si="7"/>
         <v>0.68339953579038815</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="12">
         <v>450</v>
       </c>
@@ -3055,7 +3132,7 @@
         <f>Z32</f>
         <v>2.0800000000000001E-4</v>
       </c>
-      <c r="C52" s="31">
+      <c r="C52" s="29">
         <f>AA32</f>
         <v>6.5799999999999997E-6</v>
       </c>
@@ -3063,7 +3140,7 @@
         <f>Z38</f>
         <v>1.55445386214617E-2</v>
       </c>
-      <c r="E52" s="31">
+      <c r="E52" s="29">
         <f>AA38</f>
         <v>8.0523510876941238E-4</v>
       </c>
@@ -3071,7 +3148,7 @@
         <f>Z25</f>
         <v>1.18306E-4</v>
       </c>
-      <c r="G52" s="31">
+      <c r="G52" s="29">
         <f>AA25</f>
         <v>3.3899399999999998E-6</v>
       </c>
@@ -3079,43 +3156,43 @@
         <f>Z26</f>
         <v>5.5596232727209861E-3</v>
       </c>
-      <c r="I52" s="31">
+      <c r="I52" s="29">
         <f>AA26</f>
         <v>7.1280812237153196E-4</v>
       </c>
       <c r="J52" s="14">
         <v>450</v>
       </c>
-      <c r="K52" s="32">
-        <f t="shared" si="0"/>
+      <c r="K52" s="30">
+        <f t="shared" si="1"/>
         <v>0.20800000000000002</v>
       </c>
-      <c r="L52" s="32">
-        <f t="shared" si="0"/>
+      <c r="L52" s="30">
+        <f t="shared" si="1"/>
         <v>6.5799999999999999E-3</v>
       </c>
-      <c r="M52" s="34">
-        <f t="shared" si="1"/>
+      <c r="M52" s="32">
+        <f t="shared" si="2"/>
         <v>15.544538621461699</v>
       </c>
-      <c r="N52" s="34">
-        <f t="shared" si="2"/>
+      <c r="N52" s="32">
+        <f t="shared" si="3"/>
         <v>0.8052351087694124</v>
       </c>
-      <c r="O52" s="33">
-        <f t="shared" si="3"/>
+      <c r="O52" s="31">
+        <f t="shared" si="4"/>
         <v>0.11830600000000001</v>
       </c>
-      <c r="P52" s="33">
-        <f t="shared" si="4"/>
+      <c r="P52" s="31">
+        <f t="shared" si="5"/>
         <v>3.3899399999999997E-3</v>
       </c>
-      <c r="Q52" s="34">
-        <f t="shared" si="5"/>
+      <c r="Q52" s="32">
+        <f t="shared" si="6"/>
         <v>5.5596232727209864</v>
       </c>
-      <c r="R52" s="34">
-        <f t="shared" si="6"/>
+      <c r="R52" s="32">
+        <f t="shared" si="7"/>
         <v>0.7128081223715319</v>
       </c>
     </row>
@@ -3134,24 +3211,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
04: Tex table, excel fit data
</commit_message>
<xml_diff>
--- a/04_RozpadPlazmatu/data/Rozpadgrafy.xlsx
+++ b/04_RozpadPlazmatu/data/Rozpadgrafy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\Škola Mgr\Praktikum plazma\PraktikaPlazma\04_RozpadPlazmatu\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\PraktikumPlazma\04_RozpadPlazmatu\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0E92BA-DB52-4EA4-B96E-1D00439784DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A141691F-2D6B-492E-B5C7-E06136D2EBFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="570" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25872" yWindow="4368" windowWidth="12636" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="36">
   <si>
     <t>y0</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Objemová rekomb.</t>
   </si>
   <si>
-    <t>Obě rekombinace</t>
-  </si>
-  <si>
     <t>\pm</t>
   </si>
   <si>
@@ -139,6 +136,12 @@
   </si>
   <si>
     <t>[Pa]</t>
+  </si>
+  <si>
+    <t>Kombinovaná rekombinace 1/n</t>
+  </si>
+  <si>
+    <t>Kombinovaná rekombinace ln n</t>
   </si>
 </sst>
 </file>
@@ -274,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -329,6 +332,9 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -668,17 +674,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA52"/>
+  <dimension ref="A1:AC52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X21" sqref="X21"/>
+    <sheetView tabSelected="1" topLeftCell="R28" workbookViewId="0">
+      <selection activeCell="X49" sqref="X49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
@@ -688,7 +694,7 @@
     <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>16</v>
       </c>
@@ -751,7 +757,7 @@
         <v>715.5</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>43</v>
       </c>
@@ -816,7 +822,7 @@
         <v>16.893422979581029</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>50</v>
       </c>
@@ -881,7 +887,7 @@
         <v>16.81159498480773</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>60</v>
       </c>
@@ -946,7 +952,7 @@
         <v>16.766692438187018</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>74</v>
       </c>
@@ -1011,7 +1017,7 @@
         <v>16.604609143634047</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>92</v>
       </c>
@@ -1076,7 +1082,7 @@
         <v>16.470978194037965</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>115</v>
       </c>
@@ -1141,7 +1147,7 @@
         <v>16.366104307158352</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>144</v>
       </c>
@@ -1206,7 +1212,7 @@
         <v>16.170873601587623</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>190</v>
       </c>
@@ -1271,7 +1277,7 @@
         <v>15.952423320705165</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>248</v>
       </c>
@@ -1336,7 +1342,7 @@
         <v>15.658254255367595</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>324</v>
       </c>
@@ -1401,7 +1407,7 @@
         <v>15.406426743442815</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>416</v>
       </c>
@@ -1466,7 +1472,7 @@
         <v>15.182127790498003</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>500</v>
       </c>
@@ -1531,7 +1537,7 @@
         <v>14.995171231199933</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
         <v>600</v>
       </c>
@@ -1596,7 +1602,7 @@
         <v>14.673227095141588</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="13">
         <v>700</v>
       </c>
@@ -1661,7 +1667,7 @@
         <v>14.611249394865721</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>800</v>
       </c>
@@ -1726,7 +1732,7 @@
         <v>14.500474989363804</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>3</v>
       </c>
@@ -1737,7 +1743,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>5</v>
       </c>
@@ -1745,7 +1751,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>7</v>
       </c>
@@ -1755,11 +1761,86 @@
       <c r="C20" s="12" t="s">
         <v>9</v>
       </c>
+      <c r="D20" s="22" t="s">
+        <v>14</v>
+      </c>
       <c r="E20" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="M20" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="N20" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="O20" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="P20" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q20" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="R20" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="S20" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="T20" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="U20" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="V20" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="W20" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="X20" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y20" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z20" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA20" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB20" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC20" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" s="21" t="s">
         <v>0</v>
       </c>
@@ -1770,8 +1851,11 @@
       <c r="C21" s="19">
         <v>1.39E-8</v>
       </c>
-      <c r="E21" s="21" t="s">
-        <v>0</v>
+      <c r="D21" s="19">
+        <v>-2.9999999999999999E-7</v>
+      </c>
+      <c r="E21" s="35">
+        <v>2.5699999999999999E-8</v>
       </c>
       <c r="F21" s="19">
         <v>-3.6899999999999998E-7</v>
@@ -1779,38 +1863,74 @@
       <c r="G21" s="19">
         <v>5.2399999999999999E-8</v>
       </c>
+      <c r="H21" s="19">
+        <v>-4.7899999999999999E-7</v>
+      </c>
+      <c r="I21" s="19">
+        <v>8.0999999999999997E-8</v>
+      </c>
       <c r="J21" s="19">
         <v>-2.4200000000000002E-7</v>
       </c>
       <c r="K21" s="19">
         <v>2.9000000000000002E-8</v>
       </c>
+      <c r="L21" s="19">
+        <v>-1.12E-7</v>
+      </c>
+      <c r="M21" s="19">
+        <v>2.4500000000000001E-8</v>
+      </c>
       <c r="N21" s="19">
         <v>-6.8099999999999994E-8</v>
       </c>
       <c r="O21" s="19">
         <v>1.85E-8</v>
       </c>
+      <c r="P21" s="19">
+        <v>-2.7599999999999999E-8</v>
+      </c>
+      <c r="Q21" s="19">
+        <v>5.04E-9</v>
+      </c>
       <c r="R21" s="19">
         <v>-1.29E-8</v>
       </c>
       <c r="S21" s="19">
         <v>3.2299999999999998E-9</v>
       </c>
+      <c r="T21" s="19">
+        <v>-1.9000000000000001E-8</v>
+      </c>
+      <c r="U21" s="19">
+        <v>2.3400000000000002E-9</v>
+      </c>
       <c r="V21" s="19">
         <v>-4.9199999999999997E-8</v>
       </c>
       <c r="W21" s="19">
         <v>8.9899999999999998E-9</v>
       </c>
+      <c r="X21" s="19">
+        <v>-6.0199999999999996E-8</v>
+      </c>
+      <c r="Y21" s="19">
+        <v>6.3099999999999999E-9</v>
+      </c>
       <c r="Z21" s="19">
         <v>-2.9799999999999999E-7</v>
       </c>
       <c r="AA21" s="19">
         <v>6.6600000000000001E-8</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB21" s="19">
+        <v>-2.9499999999999998E-7</v>
+      </c>
+      <c r="AC21" s="19">
+        <v>3.7499999999999998E-8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">
         <v>1</v>
       </c>
@@ -1822,8 +1942,11 @@
         <f>0.0000000118</f>
         <v>1.18E-8</v>
       </c>
-      <c r="E22" s="21" t="s">
-        <v>1</v>
+      <c r="D22" s="19">
+        <v>3.4700000000000002E-7</v>
+      </c>
+      <c r="E22" s="35">
+        <v>2.4E-8</v>
       </c>
       <c r="F22" s="19">
         <v>4.1100000000000001E-7</v>
@@ -1831,38 +1954,74 @@
       <c r="G22" s="19">
         <v>4.7799999999999998E-8</v>
       </c>
+      <c r="H22" s="19">
+        <v>5.2499999999999995E-7</v>
+      </c>
+      <c r="I22" s="19">
+        <v>7.98E-8</v>
+      </c>
       <c r="J22" s="19">
         <v>2.6600000000000003E-7</v>
       </c>
       <c r="K22" s="19">
         <v>2.59E-8</v>
       </c>
+      <c r="L22" s="19">
+        <v>1.4700000000000001E-7</v>
+      </c>
+      <c r="M22" s="19">
+        <v>2.33E-8</v>
+      </c>
       <c r="N22" s="19">
         <v>8.2399999999999997E-8</v>
       </c>
       <c r="O22" s="19">
         <v>1.26E-8</v>
       </c>
+      <c r="P22" s="19">
+        <v>5.2800000000000003E-8</v>
+      </c>
+      <c r="Q22" s="19">
+        <v>3.9600000000000004E-9</v>
+      </c>
       <c r="R22" s="19">
         <v>4.1099999999999997E-8</v>
       </c>
       <c r="S22" s="19">
         <v>2.3499999999999999E-9</v>
       </c>
+      <c r="T22" s="19">
+        <v>4.5900000000000001E-8</v>
+      </c>
+      <c r="U22" s="19">
+        <v>1.97E-9</v>
+      </c>
       <c r="V22" s="19">
         <v>7.4200000000000003E-8</v>
       </c>
       <c r="W22" s="19">
         <v>6.7999999999999997E-9</v>
       </c>
+      <c r="X22" s="19">
+        <v>8.3200000000000004E-8</v>
+      </c>
+      <c r="Y22" s="19">
+        <v>5.4700000000000003E-9</v>
+      </c>
       <c r="Z22" s="19">
         <v>3.0800000000000001E-7</v>
       </c>
       <c r="AA22" s="19">
         <v>6.1900000000000005E-8</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB22" s="19">
+        <v>3.0499999999999999E-7</v>
+      </c>
+      <c r="AC22" s="19">
+        <v>3.6099999999999999E-8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>2</v>
       </c>
@@ -1874,8 +2033,11 @@
         <f>0.0000289</f>
         <v>2.8900000000000001E-5</v>
       </c>
-      <c r="E23" s="21" t="s">
-        <v>2</v>
+      <c r="D23" s="19">
+        <v>2.2499999999999998E-3</v>
+      </c>
+      <c r="E23" s="35">
+        <v>8.7999999999999998E-5</v>
       </c>
       <c r="F23" s="19">
         <v>1.56E-3</v>
@@ -1883,38 +2045,74 @@
       <c r="G23" s="19">
         <v>1.05E-4</v>
       </c>
+      <c r="H23" s="19">
+        <v>1.34E-3</v>
+      </c>
+      <c r="I23" s="19">
+        <v>1.45E-4</v>
+      </c>
       <c r="J23" s="19">
         <v>1.8E-3</v>
       </c>
       <c r="K23" s="19">
         <v>9.48E-5</v>
       </c>
+      <c r="L23" s="19">
+        <v>2.48E-3</v>
+      </c>
+      <c r="M23" s="19">
+        <v>2.1599999999999999E-4</v>
+      </c>
       <c r="N23" s="19">
         <v>2.65E-3</v>
       </c>
       <c r="O23" s="19">
         <v>1.5799999999999999E-4</v>
       </c>
+      <c r="P23" s="19">
+        <v>3.15E-3</v>
+      </c>
+      <c r="Q23" s="19">
+        <v>9.7899999999999994E-5</v>
+      </c>
       <c r="R23" s="19">
         <v>2.2599999999999999E-3</v>
       </c>
       <c r="S23" s="19">
         <v>5.4599999999999999E-5</v>
       </c>
+      <c r="T23" s="19">
+        <v>2.15E-3</v>
+      </c>
+      <c r="U23" s="19">
+        <v>4.5500000000000001E-5</v>
+      </c>
       <c r="V23" s="19">
         <v>1.1999999999999999E-3</v>
       </c>
       <c r="W23" s="19">
         <v>4.88E-5</v>
       </c>
+      <c r="X23" s="19">
+        <v>1.14E-3</v>
+      </c>
+      <c r="Y23" s="19">
+        <v>3.82E-5</v>
+      </c>
       <c r="Z23" s="19">
         <v>3.97E-4</v>
       </c>
       <c r="AA23" s="19">
         <v>5.0899999999999997E-5</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB23" s="19">
+        <v>3.9899999999999999E-4</v>
+      </c>
+      <c r="AC23" s="19">
+        <v>3.2499999999999997E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="27" t="s">
         <v>27</v>
       </c>
@@ -1926,6 +2124,14 @@
         <f>C23*1000000</f>
         <v>28.900000000000002</v>
       </c>
+      <c r="D24" s="19">
+        <f>D23*1000000</f>
+        <v>2250</v>
+      </c>
+      <c r="E24" s="19">
+        <f>E23*1000000</f>
+        <v>88</v>
+      </c>
       <c r="F24" s="19">
         <f>F23*1000000</f>
         <v>1560</v>
@@ -1934,6 +2140,14 @@
         <f>G23*1000000</f>
         <v>105</v>
       </c>
+      <c r="H24" s="19">
+        <f>H23*1000000</f>
+        <v>1340</v>
+      </c>
+      <c r="I24" s="19">
+        <f>I23*1000000</f>
+        <v>145</v>
+      </c>
       <c r="J24" s="19">
         <f>J23*1000000</f>
         <v>1800</v>
@@ -1942,6 +2156,14 @@
         <f>K23*1000000</f>
         <v>94.8</v>
       </c>
+      <c r="L24" s="19">
+        <f>L23*1000000</f>
+        <v>2480</v>
+      </c>
+      <c r="M24" s="19">
+        <f>M23*1000000</f>
+        <v>216</v>
+      </c>
       <c r="N24" s="19">
         <f>N23*1000000</f>
         <v>2650</v>
@@ -1950,6 +2172,14 @@
         <f>O23*1000000</f>
         <v>158</v>
       </c>
+      <c r="P24" s="19">
+        <f>P23*1000000</f>
+        <v>3150</v>
+      </c>
+      <c r="Q24" s="19">
+        <f>Q23*1000000</f>
+        <v>97.899999999999991</v>
+      </c>
       <c r="R24" s="19">
         <f>R23*1000000</f>
         <v>2260</v>
@@ -1958,6 +2188,14 @@
         <f>S23*1000000</f>
         <v>54.6</v>
       </c>
+      <c r="T24" s="19">
+        <f>T23*1000000</f>
+        <v>2150</v>
+      </c>
+      <c r="U24" s="19">
+        <f>U23*1000000</f>
+        <v>45.5</v>
+      </c>
       <c r="V24" s="19">
         <f>V23*1000000</f>
         <v>1200</v>
@@ -1966,6 +2204,14 @@
         <f>W23*1000000</f>
         <v>48.8</v>
       </c>
+      <c r="X24" s="19">
+        <f>X23*1000000</f>
+        <v>1140</v>
+      </c>
+      <c r="Y24" s="19">
+        <f>Y23*1000000</f>
+        <v>38.200000000000003</v>
+      </c>
       <c r="Z24" s="19">
         <f>Z23*1000000</f>
         <v>397</v>
@@ -1974,8 +2220,16 @@
         <f>AA23*1000000</f>
         <v>50.9</v>
       </c>
-    </row>
-    <row r="25" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB24" s="19">
+        <f>AB23*1000000</f>
+        <v>399</v>
+      </c>
+      <c r="AC24" s="19">
+        <f>AC23*1000000</f>
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
         <v>24</v>
       </c>
@@ -1987,7 +2241,14 @@
         <f>C21*C24</f>
         <v>4.0171000000000002E-7</v>
       </c>
-      <c r="E25" s="28"/>
+      <c r="D25" s="28">
+        <f>-D21*D24</f>
+        <v>6.7499999999999993E-4</v>
+      </c>
+      <c r="E25" s="28">
+        <f>E21*E24</f>
+        <v>2.2615999999999997E-6</v>
+      </c>
       <c r="F25" s="28">
         <f>-F21*F24</f>
         <v>5.7563999999999998E-4</v>
@@ -1996,6 +2257,14 @@
         <f>G21*G24</f>
         <v>5.502E-6</v>
       </c>
+      <c r="H25" s="28">
+        <f>-H21*H24</f>
+        <v>6.4185999999999996E-4</v>
+      </c>
+      <c r="I25" s="28">
+        <f>I21*I24</f>
+        <v>1.1745E-5</v>
+      </c>
       <c r="J25" s="28">
         <f>-J21*J24</f>
         <v>4.3560000000000002E-4</v>
@@ -2004,6 +2273,14 @@
         <f>K21*K24</f>
         <v>2.7491999999999999E-6</v>
       </c>
+      <c r="L25" s="28">
+        <f>-L21*L24</f>
+        <v>2.7776E-4</v>
+      </c>
+      <c r="M25" s="28">
+        <f>M21*M24</f>
+        <v>5.2920000000000003E-6</v>
+      </c>
       <c r="N25" s="28">
         <f>-N21*N24</f>
         <v>1.8046499999999999E-4</v>
@@ -2012,6 +2289,14 @@
         <f>O21*O24</f>
         <v>2.9230000000000002E-6</v>
       </c>
+      <c r="P25" s="28">
+        <f>-P21*P24</f>
+        <v>8.6939999999999991E-5</v>
+      </c>
+      <c r="Q25" s="28">
+        <f>Q21*Q24</f>
+        <v>4.9341599999999992E-7</v>
+      </c>
       <c r="R25" s="28">
         <f>-R21*R24</f>
         <v>2.9153999999999999E-5</v>
@@ -2020,6 +2305,14 @@
         <f>S21*S24</f>
         <v>1.76358E-7</v>
       </c>
+      <c r="T25" s="28">
+        <f>-T21*T24</f>
+        <v>4.0850000000000004E-5</v>
+      </c>
+      <c r="U25" s="28">
+        <f>U21*U24</f>
+        <v>1.0647000000000001E-7</v>
+      </c>
       <c r="V25" s="28">
         <f>-V21*V24</f>
         <v>5.9039999999999997E-5</v>
@@ -2028,6 +2321,14 @@
         <f>W21*W24</f>
         <v>4.3871199999999994E-7</v>
       </c>
+      <c r="X25" s="28">
+        <f>-X21*X24</f>
+        <v>6.8627999999999994E-5</v>
+      </c>
+      <c r="Y25" s="28">
+        <f>Y21*Y24</f>
+        <v>2.41042E-7</v>
+      </c>
       <c r="Z25" s="28">
         <f>-Z21*Z24</f>
         <v>1.18306E-4</v>
@@ -2036,8 +2337,16 @@
         <f>AA21*AA24</f>
         <v>3.3899399999999998E-6</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB25" s="28">
+        <f>-AB21*AB24</f>
+        <v>1.17705E-4</v>
+      </c>
+      <c r="AC25" s="28">
+        <f>AC21*AC24</f>
+        <v>1.21875E-6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
         <v>25</v>
       </c>
@@ -2049,6 +2358,14 @@
         <f>C24*$B$41^2</f>
         <v>4.0471816771193075E-4</v>
       </c>
+      <c r="D26" s="28">
+        <f>D24*$B$41^2</f>
+        <v>3.1509199908368313E-2</v>
+      </c>
+      <c r="E26" s="28">
+        <f>E24*$B$41^2</f>
+        <v>1.232359818638405E-3</v>
+      </c>
       <c r="F26" s="28">
         <f>F24*$B$41^2</f>
         <v>2.1846378603135361E-2</v>
@@ -2057,6 +2374,14 @@
         <f>G24*$B$41^2</f>
         <v>1.4704293290571878E-3</v>
       </c>
+      <c r="H26" s="28">
+        <f>H24*$B$41^2</f>
+        <v>1.8765479056539348E-2</v>
+      </c>
+      <c r="I26" s="28">
+        <f>I24*$B$41^2</f>
+        <v>2.0305928829837355E-3</v>
+      </c>
       <c r="J26" s="28">
         <f>J24*$B$41^2</f>
         <v>2.5207359926694647E-2</v>
@@ -2065,6 +2390,14 @@
         <f>K24*$B$41^2</f>
         <v>1.327587622805918E-3</v>
       </c>
+      <c r="L26" s="28">
+        <f>L24*$B$41^2</f>
+        <v>3.4730140343445959E-2</v>
+      </c>
+      <c r="M26" s="28">
+        <f>M24*$B$41^2</f>
+        <v>3.0248831912033577E-3</v>
+      </c>
       <c r="N26" s="28">
         <f>N24*$B$41^2</f>
         <v>3.7110835447633786E-2</v>
@@ -2073,6 +2406,14 @@
         <f>O24*$B$41^2</f>
         <v>2.2126460380098635E-3</v>
       </c>
+      <c r="P26" s="28">
+        <f>P24*$B$41^2</f>
+        <v>4.4112879871715631E-2</v>
+      </c>
+      <c r="Q26" s="28">
+        <f>Q24*$B$41^2</f>
+        <v>1.3710002982352254E-3</v>
+      </c>
       <c r="R26" s="28">
         <f>R24*$B$41^2</f>
         <v>3.1649240796849949E-2</v>
@@ -2081,6 +2422,14 @@
         <f>S24*$B$41^2</f>
         <v>7.6462325110973769E-4</v>
       </c>
+      <c r="T26" s="28">
+        <f>T24*$B$41^2</f>
+        <v>3.0108791023551941E-2</v>
+      </c>
+      <c r="U26" s="28">
+        <f>U24*$B$41^2</f>
+        <v>6.3718604259144804E-4</v>
+      </c>
       <c r="V26" s="28">
         <f>V24*$B$41^2</f>
         <v>1.680490661779643E-2</v>
@@ -2089,6 +2438,14 @@
         <f>W24*$B$41^2</f>
         <v>6.8339953579038819E-4</v>
       </c>
+      <c r="X26" s="28">
+        <f>X24*$B$41^2</f>
+        <v>1.5964661286906611E-2</v>
+      </c>
+      <c r="Y26" s="28">
+        <f>Y24*$B$41^2</f>
+        <v>5.3495619399985313E-4</v>
+      </c>
       <c r="Z26" s="28">
         <f>Z24*$B$41^2</f>
         <v>5.5596232727209861E-3</v>
@@ -2097,12 +2454,20 @@
         <f>AA24*$B$41^2</f>
         <v>7.1280812237153196E-4</v>
       </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB26" s="28">
+        <f>AB24*$B$41^2</f>
+        <v>5.5876314504173137E-3</v>
+      </c>
+      <c r="AC26" s="28">
+        <f>AC24*$B$41^2</f>
+        <v>4.5513288756532003E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B27" s="14"/>
       <c r="E27" s="14"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B28" s="22" t="s">
         <v>8</v>
       </c>
@@ -2110,7 +2475,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" s="22" t="s">
         <v>12</v>
       </c>
@@ -2157,7 +2522,7 @@
         <v>8.4700000000000007E-9</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" s="26" t="s">
         <v>13</v>
       </c>
@@ -2204,7 +2569,7 @@
         <v>6.5799999999999998E-12</v>
       </c>
     </row>
-    <row r="31" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="22" t="s">
         <v>26</v>
       </c>
@@ -2265,7 +2630,7 @@
         <v>6.5799999999999997E-6</v>
       </c>
     </row>
-    <row r="32" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="22" t="s">
         <v>24</v>
       </c>
@@ -2327,7 +2692,7 @@
         <v>6.5799999999999997E-6</v>
       </c>
     </row>
-    <row r="33" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="22"/>
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
@@ -2345,7 +2710,7 @@
       <c r="Z33" s="19"/>
       <c r="AA33" s="19"/>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B34" s="22" t="s">
         <v>14</v>
       </c>
@@ -2354,7 +2719,7 @@
       </c>
       <c r="D34" s="19"/>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A35" s="22" t="s">
         <v>12</v>
       </c>
@@ -2402,7 +2767,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36" s="22" t="s">
         <v>13</v>
       </c>
@@ -2450,7 +2815,7 @@
         <v>5.7500000000000002E-5</v>
       </c>
     </row>
-    <row r="37" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="22" t="s">
         <v>26</v>
       </c>
@@ -2512,7 +2877,7 @@
         <v>57.5</v>
       </c>
     </row>
-    <row r="38" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="22" t="s">
         <v>25</v>
       </c>
@@ -2574,10 +2939,10 @@
         <v>8.0523510876941238E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
       <c r="D39" s="19"/>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A40" s="22" t="s">
         <v>15</v>
       </c>
@@ -2587,7 +2952,7 @@
       </c>
       <c r="D40" s="19"/>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A41" s="22" t="s">
         <v>23</v>
       </c>
@@ -2597,15 +2962,15 @@
       </c>
       <c r="D41" s="19"/>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
       <c r="D42" s="19"/>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
       <c r="D43" s="19"/>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B44" s="33" t="s">
         <v>29</v>
@@ -2616,83 +2981,119 @@
       </c>
       <c r="E44" s="34"/>
       <c r="F44" s="33" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G44" s="33"/>
       <c r="H44" s="33"/>
       <c r="I44" s="33"/>
-      <c r="J44" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="K44" s="33" t="s">
+      <c r="J44" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="K44" s="33"/>
+      <c r="L44" s="33"/>
+      <c r="M44" s="33"/>
+      <c r="N44" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="O44" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="L44" s="33"/>
-      <c r="M44" s="34" t="s">
+      <c r="P44" s="33"/>
+      <c r="Q44" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="N44" s="34"/>
-      <c r="O44" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="P44" s="33"/>
-      <c r="Q44" s="33"/>
-      <c r="R44" s="33"/>
-    </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="R44" s="34"/>
+      <c r="S44" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="T44" s="33"/>
+      <c r="U44" s="33"/>
+      <c r="V44" s="33"/>
+      <c r="W44" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="X44" s="33"/>
+      <c r="Y44" s="33"/>
+      <c r="Z44" s="33"/>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B45" s="12" t="s">
         <v>24</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D45" s="12" t="s">
         <v>25</v>
       </c>
       <c r="E45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F45" s="14" t="s">
         <v>24</v>
       </c>
       <c r="G45" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H45" s="14" t="s">
         <v>25</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J45" s="14" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="K45" s="14" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="L45" s="14" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="M45" s="14" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="N45" s="14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="O45" s="14" t="s">
         <v>24</v>
       </c>
       <c r="P45" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q45" s="14" t="s">
         <v>25</v>
       </c>
       <c r="R45" s="14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="S45" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="T45" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="U45" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="V45" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="W45" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="X45" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y45" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z45" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A46" s="12">
         <v>5</v>
       </c>
@@ -2728,43 +3129,75 @@
         <f>C26</f>
         <v>4.0471816771193075E-4</v>
       </c>
-      <c r="J46" s="14">
+      <c r="J46" s="19">
+        <f>D25</f>
+        <v>6.7499999999999993E-4</v>
+      </c>
+      <c r="K46" s="19">
+        <f>E25</f>
+        <v>2.2615999999999997E-6</v>
+      </c>
+      <c r="L46" s="19">
+        <f>D26</f>
+        <v>3.1509199908368313E-2</v>
+      </c>
+      <c r="M46" s="19">
+        <f>E26</f>
+        <v>1.232359818638405E-3</v>
+      </c>
+      <c r="N46" s="14">
         <v>5</v>
       </c>
-      <c r="K46" s="30">
-        <f t="shared" ref="K46:R46" si="0">B46*1000</f>
+      <c r="O46" s="30">
+        <f>B46*1000</f>
         <v>2.0100000000000002</v>
       </c>
-      <c r="L46" s="30">
-        <f t="shared" si="0"/>
+      <c r="P46" s="30">
+        <f>C46*1000</f>
         <v>0.11399999999999999</v>
       </c>
-      <c r="M46" s="32">
-        <f t="shared" si="0"/>
+      <c r="Q46" s="32">
+        <f>D46*1000</f>
         <v>57.276723388989502</v>
       </c>
-      <c r="N46" s="32">
-        <f t="shared" si="0"/>
+      <c r="R46" s="32">
+        <f>E46*1000</f>
         <v>2.7588055030882477</v>
       </c>
-      <c r="O46" s="25">
-        <f t="shared" si="0"/>
+      <c r="S46" s="25">
+        <f>F46*1000</f>
         <v>0.77343000000000006</v>
       </c>
-      <c r="P46" s="25">
-        <f t="shared" si="0"/>
+      <c r="T46" s="25">
+        <f>G46*1000</f>
         <v>4.0171E-4</v>
       </c>
-      <c r="Q46" s="32">
-        <f t="shared" si="0"/>
+      <c r="U46" s="32">
+        <f>H46*1000</f>
         <v>28.428300361772301</v>
       </c>
-      <c r="R46" s="32">
-        <f t="shared" si="0"/>
+      <c r="V46" s="32">
+        <f>I46*1000</f>
         <v>0.40471816771193075</v>
       </c>
-    </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="W46" s="25">
+        <f>J46*1000</f>
+        <v>0.67499999999999993</v>
+      </c>
+      <c r="X46" s="25">
+        <f>K46*1000</f>
+        <v>2.2615999999999995E-3</v>
+      </c>
+      <c r="Y46" s="32">
+        <f>L46*1000</f>
+        <v>31.509199908368313</v>
+      </c>
+      <c r="Z46" s="32">
+        <f>M46*1000</f>
+        <v>1.232359818638405</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A47" s="12">
         <v>10</v>
       </c>
@@ -2800,43 +3233,75 @@
         <f>G26</f>
         <v>1.4704293290571878E-3</v>
       </c>
-      <c r="J47" s="14">
+      <c r="J47" s="19">
+        <f>H25</f>
+        <v>6.4185999999999996E-4</v>
+      </c>
+      <c r="K47" s="19">
+        <f>I25</f>
+        <v>1.1745E-5</v>
+      </c>
+      <c r="L47" s="19">
+        <f>H26</f>
+        <v>1.8765479056539348E-2</v>
+      </c>
+      <c r="M47" s="19">
+        <f>I26</f>
+        <v>2.0305928829837355E-3</v>
+      </c>
+      <c r="N47" s="14">
         <v>10</v>
       </c>
-      <c r="K47" s="30">
-        <f t="shared" ref="K47:L52" si="1">B47*1000</f>
+      <c r="O47" s="30">
+        <f>B47*1000</f>
         <v>1.21</v>
       </c>
-      <c r="L47" s="30">
-        <f t="shared" si="1"/>
+      <c r="P47" s="30">
+        <f>C47*1000</f>
         <v>5.2199999999999996E-2</v>
       </c>
-      <c r="M47" s="32">
-        <f t="shared" ref="M47:M52" si="2">D47*1000</f>
+      <c r="Q47" s="32">
+        <f>D47*1000</f>
         <v>50.694801630352565</v>
       </c>
-      <c r="N47" s="32">
-        <f t="shared" ref="N47:N52" si="3">E47*1000</f>
+      <c r="R47" s="32">
+        <f>E47*1000</f>
         <v>3.3049649681666318</v>
       </c>
-      <c r="O47" s="31">
-        <f t="shared" ref="O47:O52" si="4">F47*1000</f>
+      <c r="S47" s="31">
+        <f>F47*1000</f>
         <v>0.57563999999999993</v>
       </c>
-      <c r="P47" s="31">
-        <f t="shared" ref="P47:P52" si="5">G47*1000</f>
+      <c r="T47" s="31">
+        <f>G47*1000</f>
         <v>5.5019999999999999E-3</v>
       </c>
-      <c r="Q47" s="32">
-        <f t="shared" ref="Q47:Q52" si="6">H47*1000</f>
+      <c r="U47" s="32">
+        <f>H47*1000</f>
         <v>21.84637860313536</v>
       </c>
-      <c r="R47" s="32">
-        <f t="shared" ref="R47:R52" si="7">I47*1000</f>
+      <c r="V47" s="32">
+        <f>I47*1000</f>
         <v>1.4704293290571879</v>
       </c>
-    </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="W47" s="31">
+        <f>J47*1000</f>
+        <v>0.64185999999999999</v>
+      </c>
+      <c r="X47" s="31">
+        <f>K47*1000</f>
+        <v>1.1745E-2</v>
+      </c>
+      <c r="Y47" s="32">
+        <f>L47*1000</f>
+        <v>18.765479056539348</v>
+      </c>
+      <c r="Z47" s="32">
+        <f>M47*1000</f>
+        <v>2.0305928829837354</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A48" s="12">
         <v>20</v>
       </c>
@@ -2872,43 +3337,75 @@
         <f>K26</f>
         <v>1.327587622805918E-3</v>
       </c>
-      <c r="J48" s="14">
+      <c r="J48" s="19">
+        <f>L25</f>
+        <v>2.7776E-4</v>
+      </c>
+      <c r="K48" s="19">
+        <f>M25</f>
+        <v>5.2920000000000003E-6</v>
+      </c>
+      <c r="L48" s="19">
+        <f>L26</f>
+        <v>3.4730140343445959E-2</v>
+      </c>
+      <c r="M48" s="19">
+        <f>M26</f>
+        <v>3.0248831912033577E-3</v>
+      </c>
+      <c r="N48" s="14">
         <v>20</v>
       </c>
-      <c r="K48" s="30">
-        <f t="shared" si="1"/>
+      <c r="O48" s="30">
+        <f>B48*1000</f>
         <v>1</v>
       </c>
-      <c r="L48" s="30">
-        <f t="shared" si="1"/>
+      <c r="P48" s="30">
+        <f>C48*1000</f>
         <v>5.6599999999999998E-2</v>
       </c>
-      <c r="M48" s="32">
-        <f t="shared" si="2"/>
+      <c r="Q48" s="32">
+        <f>D48*1000</f>
         <v>56.856600723544602</v>
       </c>
-      <c r="N48" s="32">
-        <f t="shared" si="3"/>
+      <c r="R48" s="32">
+        <f>E48*1000</f>
         <v>2.73079732539192</v>
       </c>
-      <c r="O48" s="31">
-        <f t="shared" si="4"/>
+      <c r="S48" s="31">
+        <f>F48*1000</f>
         <v>0.43560000000000004</v>
       </c>
-      <c r="P48" s="31">
-        <f t="shared" si="5"/>
+      <c r="T48" s="31">
+        <f>G48*1000</f>
         <v>2.7491999999999998E-3</v>
       </c>
-      <c r="Q48" s="32">
-        <f t="shared" si="6"/>
+      <c r="U48" s="32">
+        <f>H48*1000</f>
         <v>25.207359926694647</v>
       </c>
-      <c r="R48" s="32">
-        <f t="shared" si="7"/>
+      <c r="V48" s="32">
+        <f>I48*1000</f>
         <v>1.327587622805918</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="W48" s="31">
+        <f>J48*1000</f>
+        <v>0.27776000000000001</v>
+      </c>
+      <c r="X48" s="31">
+        <f>K48*1000</f>
+        <v>5.2920000000000007E-3</v>
+      </c>
+      <c r="Y48" s="32">
+        <f>L48*1000</f>
+        <v>34.73014034344596</v>
+      </c>
+      <c r="Z48" s="32">
+        <f>M48*1000</f>
+        <v>3.0248831912033576</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A49" s="12">
         <v>50</v>
       </c>
@@ -2944,43 +3441,75 @@
         <f>O26</f>
         <v>2.2126460380098635E-3</v>
       </c>
-      <c r="J49" s="14">
+      <c r="J49" s="19">
+        <f>P25</f>
+        <v>8.6939999999999991E-5</v>
+      </c>
+      <c r="K49" s="19">
+        <f>Q25</f>
+        <v>4.9341599999999992E-7</v>
+      </c>
+      <c r="L49" s="19">
+        <f>P26</f>
+        <v>4.4112879871715631E-2</v>
+      </c>
+      <c r="M49" s="19">
+        <f>Q26</f>
+        <v>1.3710002982352254E-3</v>
+      </c>
+      <c r="N49" s="14">
         <v>50</v>
       </c>
-      <c r="K49" s="30">
-        <f t="shared" si="1"/>
+      <c r="O49" s="30">
+        <f>B49*1000</f>
         <v>0.82199999999999995</v>
       </c>
-      <c r="L49" s="30">
-        <f t="shared" si="1"/>
+      <c r="P49" s="30">
+        <f>C49*1000</f>
         <v>7.0099999999999996E-2</v>
       </c>
-      <c r="M49" s="32">
-        <f t="shared" si="2"/>
+      <c r="Q49" s="32">
+        <f>D49*1000</f>
         <v>52.655374069095487</v>
       </c>
-      <c r="N49" s="32">
-        <f t="shared" si="3"/>
+      <c r="R49" s="32">
+        <f>E49*1000</f>
         <v>0.97748540160182573</v>
       </c>
-      <c r="O49" s="31">
-        <f t="shared" si="4"/>
+      <c r="S49" s="31">
+        <f>F49*1000</f>
         <v>0.18046499999999999</v>
       </c>
-      <c r="P49" s="31">
-        <f t="shared" si="5"/>
+      <c r="T49" s="31">
+        <f>G49*1000</f>
         <v>2.9230000000000003E-3</v>
       </c>
-      <c r="Q49" s="32">
-        <f t="shared" si="6"/>
+      <c r="U49" s="32">
+        <f>H49*1000</f>
         <v>37.110835447633789</v>
       </c>
-      <c r="R49" s="32">
-        <f t="shared" si="7"/>
+      <c r="V49" s="32">
+        <f>I49*1000</f>
         <v>2.2126460380098636</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="W49" s="31">
+        <f>J49*1000</f>
+        <v>8.693999999999999E-2</v>
+      </c>
+      <c r="X49" s="25">
+        <f>K49*1000</f>
+        <v>4.9341599999999989E-4</v>
+      </c>
+      <c r="Y49" s="32">
+        <f>L49*1000</f>
+        <v>44.112879871715634</v>
+      </c>
+      <c r="Z49" s="32">
+        <f>M49*1000</f>
+        <v>1.3710002982352254</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A50" s="12">
         <v>100</v>
       </c>
@@ -3016,43 +3545,75 @@
         <f>S26</f>
         <v>7.6462325110973769E-4</v>
       </c>
-      <c r="J50" s="14">
+      <c r="J50" s="19">
+        <f>T25</f>
+        <v>4.0850000000000004E-5</v>
+      </c>
+      <c r="K50" s="19">
+        <f>U25</f>
+        <v>1.0647000000000001E-7</v>
+      </c>
+      <c r="L50" s="19">
+        <f>T26</f>
+        <v>3.0108791023551941E-2</v>
+      </c>
+      <c r="M50" s="19">
+        <f>U26</f>
+        <v>6.3718604259144804E-4</v>
+      </c>
+      <c r="N50" s="14">
         <v>100</v>
       </c>
-      <c r="K50" s="30">
-        <f t="shared" si="1"/>
+      <c r="O50" s="30">
+        <f>B50*1000</f>
         <v>0.30299999999999999</v>
       </c>
-      <c r="L50" s="30">
-        <f t="shared" si="1"/>
+      <c r="P50" s="30">
+        <f>C50*1000</f>
         <v>2.0999999999999998E-2</v>
       </c>
-      <c r="M50" s="32">
-        <f t="shared" si="2"/>
+      <c r="Q50" s="32">
+        <f>D50*1000</f>
         <v>36.130549228262332</v>
       </c>
-      <c r="N50" s="32">
-        <f t="shared" si="3"/>
+      <c r="R50" s="32">
+        <f>E50*1000</f>
         <v>0.45793370533495281</v>
       </c>
-      <c r="O50" s="25">
-        <f t="shared" si="4"/>
+      <c r="S50" s="25">
+        <f>F50*1000</f>
         <v>2.9153999999999999E-2</v>
       </c>
-      <c r="P50" s="25">
-        <f t="shared" si="5"/>
+      <c r="T50" s="25">
+        <f>G50*1000</f>
         <v>1.7635799999999999E-4</v>
       </c>
-      <c r="Q50" s="32">
-        <f t="shared" si="6"/>
+      <c r="U50" s="32">
+        <f>H50*1000</f>
         <v>31.649240796849949</v>
       </c>
-      <c r="R50" s="32">
-        <f t="shared" si="7"/>
+      <c r="V50" s="32">
+        <f>I50*1000</f>
         <v>0.76462325110973772</v>
       </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="W50" s="25">
+        <f>J50*1000</f>
+        <v>4.0850000000000004E-2</v>
+      </c>
+      <c r="X50" s="25">
+        <f>K50*1000</f>
+        <v>1.0647000000000002E-4</v>
+      </c>
+      <c r="Y50" s="32">
+        <f>L50*1000</f>
+        <v>30.108791023551941</v>
+      </c>
+      <c r="Z50" s="32">
+        <f>M50*1000</f>
+        <v>0.63718604259144807</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A51" s="12">
         <v>200</v>
       </c>
@@ -3088,43 +3649,75 @@
         <f>W26</f>
         <v>6.8339953579038819E-4</v>
       </c>
-      <c r="J51" s="14">
+      <c r="J51" s="19">
+        <f>X25</f>
+        <v>6.8627999999999994E-5</v>
+      </c>
+      <c r="K51" s="19">
+        <f>Y25</f>
+        <v>2.41042E-7</v>
+      </c>
+      <c r="L51" s="19">
+        <f>X26</f>
+        <v>1.5964661286906611E-2</v>
+      </c>
+      <c r="M51" s="19">
+        <f>Y26</f>
+        <v>5.3495619399985313E-4</v>
+      </c>
+      <c r="N51" s="14">
         <v>200</v>
       </c>
-      <c r="K51" s="30">
-        <f t="shared" si="1"/>
+      <c r="O51" s="30">
+        <f>B51*1000</f>
         <v>0.27399999999999997</v>
       </c>
-      <c r="L51" s="30">
-        <f t="shared" si="1"/>
+      <c r="P51" s="30">
+        <f>C51*1000</f>
         <v>1.5800000000000002E-2</v>
       </c>
-      <c r="M51" s="32">
-        <f t="shared" si="2"/>
+      <c r="Q51" s="32">
+        <f>D51*1000</f>
         <v>23.246787487951728</v>
       </c>
-      <c r="N51" s="32">
-        <f t="shared" si="3"/>
+      <c r="R51" s="32">
+        <f>E51*1000</f>
         <v>0.58957214050769158</v>
       </c>
-      <c r="O51" s="25">
-        <f t="shared" si="4"/>
+      <c r="S51" s="25">
+        <f>F51*1000</f>
         <v>5.9039999999999995E-2</v>
       </c>
-      <c r="P51" s="25">
-        <f t="shared" si="5"/>
+      <c r="T51" s="25">
+        <f>G51*1000</f>
         <v>4.3871199999999996E-4</v>
       </c>
-      <c r="Q51" s="32">
-        <f t="shared" si="6"/>
+      <c r="U51" s="32">
+        <f>H51*1000</f>
         <v>16.80490661779643</v>
       </c>
-      <c r="R51" s="32">
-        <f t="shared" si="7"/>
+      <c r="V51" s="32">
+        <f>I51*1000</f>
         <v>0.68339953579038815</v>
       </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="W51" s="25">
+        <f>J51*1000</f>
+        <v>6.8627999999999995E-2</v>
+      </c>
+      <c r="X51" s="25">
+        <f>K51*1000</f>
+        <v>2.4104199999999999E-4</v>
+      </c>
+      <c r="Y51" s="32">
+        <f>L51*1000</f>
+        <v>15.964661286906612</v>
+      </c>
+      <c r="Z51" s="32">
+        <f>M51*1000</f>
+        <v>0.53495619399985317</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A52" s="12">
         <v>450</v>
       </c>
@@ -3160,50 +3753,84 @@
         <f>AA26</f>
         <v>7.1280812237153196E-4</v>
       </c>
-      <c r="J52" s="14">
+      <c r="J52" s="19">
+        <f>AB25</f>
+        <v>1.17705E-4</v>
+      </c>
+      <c r="K52" s="19">
+        <f>AC25</f>
+        <v>1.21875E-6</v>
+      </c>
+      <c r="L52" s="19">
+        <f>AB26</f>
+        <v>5.5876314504173137E-3</v>
+      </c>
+      <c r="M52" s="19">
+        <f>AC26</f>
+        <v>4.5513288756532003E-4</v>
+      </c>
+      <c r="N52" s="14">
         <v>450</v>
       </c>
-      <c r="K52" s="30">
-        <f t="shared" si="1"/>
+      <c r="O52" s="30">
+        <f>B52*1000</f>
         <v>0.20800000000000002</v>
       </c>
-      <c r="L52" s="30">
-        <f t="shared" si="1"/>
+      <c r="P52" s="30">
+        <f>C52*1000</f>
         <v>6.5799999999999999E-3</v>
       </c>
-      <c r="M52" s="32">
-        <f t="shared" si="2"/>
+      <c r="Q52" s="32">
+        <f>D52*1000</f>
         <v>15.544538621461699</v>
       </c>
-      <c r="N52" s="32">
-        <f t="shared" si="3"/>
+      <c r="R52" s="32">
+        <f>E52*1000</f>
         <v>0.8052351087694124</v>
       </c>
-      <c r="O52" s="31">
-        <f t="shared" si="4"/>
+      <c r="S52" s="31">
+        <f>F52*1000</f>
         <v>0.11830600000000001</v>
       </c>
-      <c r="P52" s="31">
-        <f t="shared" si="5"/>
+      <c r="T52" s="31">
+        <f>G52*1000</f>
         <v>3.3899399999999997E-3</v>
       </c>
-      <c r="Q52" s="32">
-        <f t="shared" si="6"/>
+      <c r="U52" s="32">
+        <f>H52*1000</f>
         <v>5.5596232727209864</v>
       </c>
-      <c r="R52" s="32">
-        <f t="shared" si="7"/>
+      <c r="V52" s="32">
+        <f>I52*1000</f>
         <v>0.7128081223715319</v>
       </c>
+      <c r="W52" s="31">
+        <f>J52*1000</f>
+        <v>0.117705</v>
+      </c>
+      <c r="X52" s="31">
+        <f>K52*1000</f>
+        <v>1.21875E-3</v>
+      </c>
+      <c r="Y52" s="32">
+        <f>L52*1000</f>
+        <v>5.5876314504173141</v>
+      </c>
+      <c r="Z52" s="32">
+        <f>M52*1000</f>
+        <v>0.45513288756532005</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="O44:R44"/>
+  <mergeCells count="8">
+    <mergeCell ref="W44:Z44"/>
+    <mergeCell ref="S44:V44"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="F44:I44"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="O44:P44"/>
+    <mergeCell ref="Q44:R44"/>
+    <mergeCell ref="J44:M44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3216,7 +3843,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3228,7 +3855,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
04: Graphs remade by 9 orders
</commit_message>
<xml_diff>
--- a/04_RozpadPlazmatu/data/Rozpadgrafy.xlsx
+++ b/04_RozpadPlazmatu/data/Rozpadgrafy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\PraktikumPlazma\04_RozpadPlazmatu\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A141691F-2D6B-492E-B5C7-E06136D2EBFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61863303-33AE-4513-8298-BC4E5B37A503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25872" yWindow="4368" windowWidth="12636" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="39">
   <si>
     <t>y0</t>
   </si>
@@ -143,6 +143,15 @@
   <si>
     <t>Kombinovaná rekombinace ln n</t>
   </si>
+  <si>
+    <t>y0 corrected</t>
+  </si>
+  <si>
+    <t>A not updated</t>
+  </si>
+  <si>
+    <t>Intercept not updated</t>
+  </si>
 </sst>
 </file>
 
@@ -154,7 +163,7 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,6 +195,23 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -277,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -327,14 +353,23 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -674,10 +709,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC52"/>
+  <dimension ref="A1:AC53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R28" workbookViewId="0">
-      <selection activeCell="X49" sqref="X49"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A10" sqref="A10"/>
+      <selection pane="topRight" activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1742,6 +1779,9 @@
       <c r="C18" s="23" t="s">
         <v>10</v>
       </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="19" spans="1:29" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
@@ -1854,7 +1894,7 @@
       <c r="D21" s="19">
         <v>-2.9999999999999999E-7</v>
       </c>
-      <c r="E21" s="35">
+      <c r="E21" s="33">
         <v>2.5699999999999999E-8</v>
       </c>
       <c r="F21" s="19">
@@ -1864,10 +1904,10 @@
         <v>5.2399999999999999E-8</v>
       </c>
       <c r="H21" s="19">
-        <v>-4.7899999999999999E-7</v>
+        <v>-4.5400000000000002E-7</v>
       </c>
       <c r="I21" s="19">
-        <v>8.0999999999999997E-8</v>
+        <v>5.9599999999999998E-8</v>
       </c>
       <c r="J21" s="19">
         <v>-2.4200000000000002E-7</v>
@@ -1945,7 +1985,7 @@
       <c r="D22" s="19">
         <v>3.4700000000000002E-7</v>
       </c>
-      <c r="E22" s="35">
+      <c r="E22" s="33">
         <v>2.4E-8</v>
       </c>
       <c r="F22" s="19">
@@ -1955,10 +1995,10 @@
         <v>4.7799999999999998E-8</v>
       </c>
       <c r="H22" s="19">
-        <v>5.2499999999999995E-7</v>
+        <v>5.0100000000000005E-7</v>
       </c>
       <c r="I22" s="19">
-        <v>7.98E-8</v>
+        <v>5.84E-8</v>
       </c>
       <c r="J22" s="19">
         <v>2.6600000000000003E-7</v>
@@ -2036,7 +2076,7 @@
       <c r="D23" s="19">
         <v>2.2499999999999998E-3</v>
       </c>
-      <c r="E23" s="35">
+      <c r="E23" s="33">
         <v>8.7999999999999998E-5</v>
       </c>
       <c r="F23" s="19">
@@ -2046,10 +2086,10 @@
         <v>1.05E-4</v>
       </c>
       <c r="H23" s="19">
-        <v>1.34E-3</v>
+        <v>1.39E-3</v>
       </c>
       <c r="I23" s="19">
-        <v>1.45E-4</v>
+        <v>1.0900000000000001E-4</v>
       </c>
       <c r="J23" s="19">
         <v>1.8E-3</v>
@@ -2112,1725 +2152,1844 @@
         <v>3.2499999999999997E-5</v>
       </c>
     </row>
-    <row r="24" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="27" t="s">
+    <row r="24" spans="1:29" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="37">
+        <f>B21*0.000000001</f>
+        <v>-3.8100000000000003E-16</v>
+      </c>
+      <c r="C24" s="37">
+        <f t="shared" ref="C24:AC24" si="0">C21*0.000000001</f>
+        <v>1.3900000000000002E-17</v>
+      </c>
+      <c r="D24" s="37">
+        <f t="shared" si="0"/>
+        <v>-2.9999999999999999E-16</v>
+      </c>
+      <c r="E24" s="37">
+        <f t="shared" si="0"/>
+        <v>2.57E-17</v>
+      </c>
+      <c r="F24" s="37">
+        <f t="shared" si="0"/>
+        <v>-3.6899999999999998E-16</v>
+      </c>
+      <c r="G24" s="37">
+        <f t="shared" si="0"/>
+        <v>5.2400000000000005E-17</v>
+      </c>
+      <c r="H24" s="37">
+        <f t="shared" si="0"/>
+        <v>-4.5400000000000008E-16</v>
+      </c>
+      <c r="I24" s="37">
+        <f t="shared" si="0"/>
+        <v>5.9599999999999997E-17</v>
+      </c>
+      <c r="J24" s="37">
+        <f t="shared" si="0"/>
+        <v>-2.4200000000000004E-16</v>
+      </c>
+      <c r="K24" s="37">
+        <f t="shared" si="0"/>
+        <v>2.9000000000000003E-17</v>
+      </c>
+      <c r="L24" s="37">
+        <f t="shared" si="0"/>
+        <v>-1.12E-16</v>
+      </c>
+      <c r="M24" s="37">
+        <f t="shared" si="0"/>
+        <v>2.4500000000000004E-17</v>
+      </c>
+      <c r="N24" s="37">
+        <f t="shared" si="0"/>
+        <v>-6.81E-17</v>
+      </c>
+      <c r="O24" s="37">
+        <f t="shared" si="0"/>
+        <v>1.8500000000000002E-17</v>
+      </c>
+      <c r="P24" s="37">
+        <f t="shared" si="0"/>
+        <v>-2.7600000000000001E-17</v>
+      </c>
+      <c r="Q24" s="37">
+        <f t="shared" si="0"/>
+        <v>5.0400000000000001E-18</v>
+      </c>
+      <c r="R24" s="37">
+        <f t="shared" si="0"/>
+        <v>-1.2900000000000001E-17</v>
+      </c>
+      <c r="S24" s="37">
+        <f t="shared" si="0"/>
+        <v>3.2300000000000001E-18</v>
+      </c>
+      <c r="T24" s="37">
+        <f t="shared" si="0"/>
+        <v>-1.9000000000000004E-17</v>
+      </c>
+      <c r="U24" s="37">
+        <f t="shared" si="0"/>
+        <v>2.3400000000000003E-18</v>
+      </c>
+      <c r="V24" s="37">
+        <f t="shared" si="0"/>
+        <v>-4.9200000000000003E-17</v>
+      </c>
+      <c r="W24" s="37">
+        <f t="shared" si="0"/>
+        <v>8.9900000000000007E-18</v>
+      </c>
+      <c r="X24" s="37">
+        <f t="shared" si="0"/>
+        <v>-6.0199999999999997E-17</v>
+      </c>
+      <c r="Y24" s="37">
+        <f t="shared" si="0"/>
+        <v>6.3100000000000003E-18</v>
+      </c>
+      <c r="Z24" s="37">
+        <f t="shared" si="0"/>
+        <v>-2.9800000000000001E-16</v>
+      </c>
+      <c r="AA24" s="37">
+        <f t="shared" si="0"/>
+        <v>6.66E-17</v>
+      </c>
+      <c r="AB24" s="37">
+        <f t="shared" si="0"/>
+        <v>-2.9500000000000001E-16</v>
+      </c>
+      <c r="AC24" s="37">
+        <f t="shared" si="0"/>
+        <v>3.7499999999999999E-17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="19">
-        <f>B23*1000000</f>
+      <c r="B25" s="19">
+        <f t="shared" ref="B25:AC25" si="1">B23*1000000</f>
         <v>2030.0000000000002</v>
       </c>
-      <c r="C24" s="19">
-        <f>C23*1000000</f>
+      <c r="C25" s="19">
+        <f t="shared" si="1"/>
         <v>28.900000000000002</v>
       </c>
-      <c r="D24" s="19">
-        <f>D23*1000000</f>
+      <c r="D25" s="19">
+        <f t="shared" si="1"/>
         <v>2250</v>
       </c>
-      <c r="E24" s="19">
-        <f>E23*1000000</f>
+      <c r="E25" s="19">
+        <f t="shared" si="1"/>
         <v>88</v>
       </c>
-      <c r="F24" s="19">
-        <f>F23*1000000</f>
+      <c r="F25" s="19">
+        <f t="shared" si="1"/>
         <v>1560</v>
       </c>
-      <c r="G24" s="19">
-        <f>G23*1000000</f>
+      <c r="G25" s="19">
+        <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="H24" s="19">
-        <f>H23*1000000</f>
-        <v>1340</v>
-      </c>
-      <c r="I24" s="19">
-        <f>I23*1000000</f>
-        <v>145</v>
-      </c>
-      <c r="J24" s="19">
-        <f>J23*1000000</f>
+      <c r="H25" s="19">
+        <f t="shared" si="1"/>
+        <v>1390</v>
+      </c>
+      <c r="I25" s="19">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="J25" s="19">
+        <f t="shared" si="1"/>
         <v>1800</v>
       </c>
-      <c r="K24" s="19">
-        <f>K23*1000000</f>
+      <c r="K25" s="19">
+        <f t="shared" si="1"/>
         <v>94.8</v>
       </c>
-      <c r="L24" s="19">
-        <f>L23*1000000</f>
+      <c r="L25" s="19">
+        <f t="shared" si="1"/>
         <v>2480</v>
       </c>
-      <c r="M24" s="19">
-        <f>M23*1000000</f>
+      <c r="M25" s="19">
+        <f t="shared" si="1"/>
         <v>216</v>
       </c>
-      <c r="N24" s="19">
-        <f>N23*1000000</f>
+      <c r="N25" s="19">
+        <f t="shared" si="1"/>
         <v>2650</v>
       </c>
-      <c r="O24" s="19">
-        <f>O23*1000000</f>
+      <c r="O25" s="19">
+        <f t="shared" si="1"/>
         <v>158</v>
       </c>
-      <c r="P24" s="19">
-        <f>P23*1000000</f>
+      <c r="P25" s="19">
+        <f t="shared" si="1"/>
         <v>3150</v>
       </c>
-      <c r="Q24" s="19">
-        <f>Q23*1000000</f>
+      <c r="Q25" s="19">
+        <f t="shared" si="1"/>
         <v>97.899999999999991</v>
       </c>
-      <c r="R24" s="19">
-        <f>R23*1000000</f>
+      <c r="R25" s="19">
+        <f t="shared" si="1"/>
         <v>2260</v>
       </c>
-      <c r="S24" s="19">
-        <f>S23*1000000</f>
+      <c r="S25" s="19">
+        <f t="shared" si="1"/>
         <v>54.6</v>
       </c>
-      <c r="T24" s="19">
-        <f>T23*1000000</f>
+      <c r="T25" s="19">
+        <f t="shared" si="1"/>
         <v>2150</v>
       </c>
-      <c r="U24" s="19">
-        <f>U23*1000000</f>
+      <c r="U25" s="19">
+        <f t="shared" si="1"/>
         <v>45.5</v>
       </c>
-      <c r="V24" s="19">
-        <f>V23*1000000</f>
+      <c r="V25" s="19">
+        <f t="shared" si="1"/>
         <v>1200</v>
       </c>
-      <c r="W24" s="19">
-        <f>W23*1000000</f>
+      <c r="W25" s="19">
+        <f t="shared" si="1"/>
         <v>48.8</v>
       </c>
-      <c r="X24" s="19">
-        <f>X23*1000000</f>
+      <c r="X25" s="19">
+        <f t="shared" si="1"/>
         <v>1140</v>
       </c>
-      <c r="Y24" s="19">
-        <f>Y23*1000000</f>
+      <c r="Y25" s="19">
+        <f t="shared" si="1"/>
         <v>38.200000000000003</v>
       </c>
-      <c r="Z24" s="19">
-        <f>Z23*1000000</f>
+      <c r="Z25" s="19">
+        <f t="shared" si="1"/>
         <v>397</v>
       </c>
-      <c r="AA24" s="19">
-        <f>AA23*1000000</f>
+      <c r="AA25" s="19">
+        <f t="shared" si="1"/>
         <v>50.9</v>
       </c>
-      <c r="AB24" s="19">
-        <f>AB23*1000000</f>
+      <c r="AB25" s="19">
+        <f t="shared" si="1"/>
         <v>399</v>
       </c>
-      <c r="AC24" s="19">
-        <f>AC23*1000000</f>
+      <c r="AC25" s="19">
+        <f t="shared" si="1"/>
         <v>32.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:29" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="28">
-        <f>-B21*B24</f>
-        <v>7.7343000000000008E-4</v>
-      </c>
-      <c r="C25" s="28">
-        <f>C21*C24</f>
-        <v>4.0171000000000002E-7</v>
-      </c>
-      <c r="D25" s="28">
-        <f>-D21*D24</f>
-        <v>6.7499999999999993E-4</v>
-      </c>
-      <c r="E25" s="28">
-        <f>E21*E24</f>
-        <v>2.2615999999999997E-6</v>
-      </c>
-      <c r="F25" s="28">
-        <f>-F21*F24</f>
-        <v>5.7563999999999998E-4</v>
-      </c>
-      <c r="G25" s="28">
-        <f>G21*G24</f>
-        <v>5.502E-6</v>
-      </c>
-      <c r="H25" s="28">
-        <f>-H21*H24</f>
-        <v>6.4185999999999996E-4</v>
-      </c>
-      <c r="I25" s="28">
-        <f>I21*I24</f>
-        <v>1.1745E-5</v>
-      </c>
-      <c r="J25" s="28">
-        <f>-J21*J24</f>
-        <v>4.3560000000000002E-4</v>
-      </c>
-      <c r="K25" s="28">
-        <f>K21*K24</f>
-        <v>2.7491999999999999E-6</v>
-      </c>
-      <c r="L25" s="28">
-        <f>-L21*L24</f>
-        <v>2.7776E-4</v>
-      </c>
-      <c r="M25" s="28">
-        <f>M21*M24</f>
-        <v>5.2920000000000003E-6</v>
-      </c>
-      <c r="N25" s="28">
-        <f>-N21*N24</f>
-        <v>1.8046499999999999E-4</v>
-      </c>
-      <c r="O25" s="28">
-        <f>O21*O24</f>
-        <v>2.9230000000000002E-6</v>
-      </c>
-      <c r="P25" s="28">
-        <f>-P21*P24</f>
-        <v>8.6939999999999991E-5</v>
-      </c>
-      <c r="Q25" s="28">
-        <f>Q21*Q24</f>
-        <v>4.9341599999999992E-7</v>
-      </c>
-      <c r="R25" s="28">
-        <f>-R21*R24</f>
-        <v>2.9153999999999999E-5</v>
-      </c>
-      <c r="S25" s="28">
-        <f>S21*S24</f>
-        <v>1.76358E-7</v>
-      </c>
-      <c r="T25" s="28">
-        <f>-T21*T24</f>
-        <v>4.0850000000000004E-5</v>
-      </c>
-      <c r="U25" s="28">
-        <f>U21*U24</f>
-        <v>1.0647000000000001E-7</v>
-      </c>
-      <c r="V25" s="28">
-        <f>-V21*V24</f>
-        <v>5.9039999999999997E-5</v>
-      </c>
-      <c r="W25" s="28">
-        <f>W21*W24</f>
-        <v>4.3871199999999994E-7</v>
-      </c>
-      <c r="X25" s="28">
-        <f>-X21*X24</f>
-        <v>6.8627999999999994E-5</v>
-      </c>
-      <c r="Y25" s="28">
-        <f>Y21*Y24</f>
-        <v>2.41042E-7</v>
-      </c>
-      <c r="Z25" s="28">
-        <f>-Z21*Z24</f>
-        <v>1.18306E-4</v>
-      </c>
-      <c r="AA25" s="28">
-        <f>AA21*AA24</f>
-        <v>3.3899399999999998E-6</v>
-      </c>
-      <c r="AB25" s="28">
-        <f>-AB21*AB24</f>
-        <v>1.17705E-4</v>
-      </c>
-      <c r="AC25" s="28">
-        <f>AC21*AC24</f>
-        <v>1.21875E-6</v>
       </c>
     </row>
     <row r="26" spans="1:29" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="28">
+        <f>-B24*B25</f>
+        <v>7.7343000000000017E-13</v>
+      </c>
+      <c r="C26" s="28">
+        <f>C24*C25</f>
+        <v>4.0171000000000007E-16</v>
+      </c>
+      <c r="D26" s="28">
+        <f>-D24*D25</f>
+        <v>6.7499999999999995E-13</v>
+      </c>
+      <c r="E26" s="28">
+        <f>E24*E25</f>
+        <v>2.2615999999999999E-15</v>
+      </c>
+      <c r="F26" s="28">
+        <f>-F24*F25</f>
+        <v>5.7563999999999996E-13</v>
+      </c>
+      <c r="G26" s="28">
+        <f>G24*G25</f>
+        <v>5.5020000000000007E-15</v>
+      </c>
+      <c r="H26" s="28">
+        <f>-H24*H25</f>
+        <v>6.3106000000000014E-13</v>
+      </c>
+      <c r="I26" s="28">
+        <f>I24*I25</f>
+        <v>6.4963999999999996E-15</v>
+      </c>
+      <c r="J26" s="28">
+        <f>-J24*J25</f>
+        <v>4.3560000000000008E-13</v>
+      </c>
+      <c r="K26" s="28">
+        <f>K24*K25</f>
+        <v>2.7492000000000002E-15</v>
+      </c>
+      <c r="L26" s="28">
+        <f>-L24*L25</f>
+        <v>2.7775999999999997E-13</v>
+      </c>
+      <c r="M26" s="28">
+        <f>M24*M25</f>
+        <v>5.2920000000000008E-15</v>
+      </c>
+      <c r="N26" s="28">
+        <f>-N24*N25</f>
+        <v>1.80465E-13</v>
+      </c>
+      <c r="O26" s="28">
+        <f>O24*O25</f>
+        <v>2.9230000000000004E-15</v>
+      </c>
+      <c r="P26" s="28">
+        <f>-P24*P25</f>
+        <v>8.6940000000000006E-14</v>
+      </c>
+      <c r="Q26" s="28">
+        <f>Q24*Q25</f>
+        <v>4.9341599999999997E-16</v>
+      </c>
+      <c r="R26" s="28">
+        <f>-R24*R25</f>
+        <v>2.9154E-14</v>
+      </c>
+      <c r="S26" s="28">
+        <f>S24*S25</f>
+        <v>1.7635800000000001E-16</v>
+      </c>
+      <c r="T26" s="28">
+        <f>-T24*T25</f>
+        <v>4.085000000000001E-14</v>
+      </c>
+      <c r="U26" s="28">
+        <f>U24*U25</f>
+        <v>1.0647000000000001E-16</v>
+      </c>
+      <c r="V26" s="28">
+        <f>-V24*V25</f>
+        <v>5.9040000000000006E-14</v>
+      </c>
+      <c r="W26" s="28">
+        <f>W24*W25</f>
+        <v>4.3871200000000002E-16</v>
+      </c>
+      <c r="X26" s="28">
+        <f>-X24*X25</f>
+        <v>6.8628000000000001E-14</v>
+      </c>
+      <c r="Y26" s="28">
+        <f>Y24*Y25</f>
+        <v>2.4104200000000005E-16</v>
+      </c>
+      <c r="Z26" s="28">
+        <f>-Z24*Z25</f>
+        <v>1.1830600000000002E-13</v>
+      </c>
+      <c r="AA26" s="28">
+        <f>AA24*AA25</f>
+        <v>3.38994E-15</v>
+      </c>
+      <c r="AB26" s="28">
+        <f>-AB24*AB25</f>
+        <v>1.17705E-13</v>
+      </c>
+      <c r="AC26" s="28">
+        <f>AC24*AC25</f>
+        <v>1.2187499999999999E-15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="28">
-        <f>B24*$B$41^2</f>
+      <c r="B27" s="28">
+        <f t="shared" ref="B27:AC27" si="2">B25*$B$42^2</f>
         <v>2.84283003617723E-2</v>
       </c>
-      <c r="C26" s="28">
-        <f>C24*$B$41^2</f>
+      <c r="C27" s="28">
+        <f t="shared" si="2"/>
         <v>4.0471816771193075E-4</v>
       </c>
-      <c r="D26" s="28">
-        <f>D24*$B$41^2</f>
+      <c r="D27" s="28">
+        <f t="shared" si="2"/>
         <v>3.1509199908368313E-2</v>
       </c>
-      <c r="E26" s="28">
-        <f>E24*$B$41^2</f>
+      <c r="E27" s="28">
+        <f t="shared" si="2"/>
         <v>1.232359818638405E-3</v>
       </c>
-      <c r="F26" s="28">
-        <f>F24*$B$41^2</f>
+      <c r="F27" s="28">
+        <f t="shared" si="2"/>
         <v>2.1846378603135361E-2</v>
       </c>
-      <c r="G26" s="28">
-        <f>G24*$B$41^2</f>
+      <c r="G27" s="28">
+        <f t="shared" si="2"/>
         <v>1.4704293290571878E-3</v>
       </c>
-      <c r="H26" s="28">
-        <f>H24*$B$41^2</f>
-        <v>1.8765479056539348E-2</v>
-      </c>
-      <c r="I26" s="28">
-        <f>I24*$B$41^2</f>
-        <v>2.0305928829837355E-3</v>
-      </c>
-      <c r="J26" s="28">
-        <f>J24*$B$41^2</f>
+      <c r="H27" s="28">
+        <f t="shared" si="2"/>
+        <v>1.9465683498947534E-2</v>
+      </c>
+      <c r="I27" s="28">
+        <f t="shared" si="2"/>
+        <v>1.5264456844498425E-3</v>
+      </c>
+      <c r="J27" s="28">
+        <f t="shared" si="2"/>
         <v>2.5207359926694647E-2</v>
       </c>
-      <c r="K26" s="28">
-        <f>K24*$B$41^2</f>
+      <c r="K27" s="28">
+        <f t="shared" si="2"/>
         <v>1.327587622805918E-3</v>
       </c>
-      <c r="L26" s="28">
-        <f>L24*$B$41^2</f>
+      <c r="L27" s="28">
+        <f t="shared" si="2"/>
         <v>3.4730140343445959E-2</v>
       </c>
-      <c r="M26" s="28">
-        <f>M24*$B$41^2</f>
+      <c r="M27" s="28">
+        <f t="shared" si="2"/>
         <v>3.0248831912033577E-3</v>
       </c>
-      <c r="N26" s="28">
-        <f>N24*$B$41^2</f>
+      <c r="N27" s="28">
+        <f t="shared" si="2"/>
         <v>3.7110835447633786E-2</v>
       </c>
-      <c r="O26" s="28">
-        <f>O24*$B$41^2</f>
+      <c r="O27" s="28">
+        <f t="shared" si="2"/>
         <v>2.2126460380098635E-3</v>
       </c>
-      <c r="P26" s="28">
-        <f>P24*$B$41^2</f>
+      <c r="P27" s="28">
+        <f t="shared" si="2"/>
         <v>4.4112879871715631E-2</v>
       </c>
-      <c r="Q26" s="28">
-        <f>Q24*$B$41^2</f>
+      <c r="Q27" s="28">
+        <f t="shared" si="2"/>
         <v>1.3710002982352254E-3</v>
       </c>
-      <c r="R26" s="28">
-        <f>R24*$B$41^2</f>
+      <c r="R27" s="28">
+        <f t="shared" si="2"/>
         <v>3.1649240796849949E-2</v>
       </c>
-      <c r="S26" s="28">
-        <f>S24*$B$41^2</f>
+      <c r="S27" s="28">
+        <f t="shared" si="2"/>
         <v>7.6462325110973769E-4</v>
       </c>
-      <c r="T26" s="28">
-        <f>T24*$B$41^2</f>
+      <c r="T27" s="28">
+        <f t="shared" si="2"/>
         <v>3.0108791023551941E-2</v>
       </c>
-      <c r="U26" s="28">
-        <f>U24*$B$41^2</f>
+      <c r="U27" s="28">
+        <f t="shared" si="2"/>
         <v>6.3718604259144804E-4</v>
       </c>
-      <c r="V26" s="28">
-        <f>V24*$B$41^2</f>
+      <c r="V27" s="28">
+        <f t="shared" si="2"/>
         <v>1.680490661779643E-2</v>
       </c>
-      <c r="W26" s="28">
-        <f>W24*$B$41^2</f>
+      <c r="W27" s="28">
+        <f t="shared" si="2"/>
         <v>6.8339953579038819E-4</v>
       </c>
-      <c r="X26" s="28">
-        <f>X24*$B$41^2</f>
+      <c r="X27" s="28">
+        <f t="shared" si="2"/>
         <v>1.5964661286906611E-2</v>
       </c>
-      <c r="Y26" s="28">
-        <f>Y24*$B$41^2</f>
+      <c r="Y27" s="28">
+        <f t="shared" si="2"/>
         <v>5.3495619399985313E-4</v>
       </c>
-      <c r="Z26" s="28">
-        <f>Z24*$B$41^2</f>
+      <c r="Z27" s="28">
+        <f t="shared" si="2"/>
         <v>5.5596232727209861E-3</v>
       </c>
-      <c r="AA26" s="28">
-        <f>AA24*$B$41^2</f>
+      <c r="AA27" s="28">
+        <f t="shared" si="2"/>
         <v>7.1280812237153196E-4</v>
       </c>
-      <c r="AB26" s="28">
-        <f>AB24*$B$41^2</f>
+      <c r="AB27" s="28">
+        <f t="shared" si="2"/>
         <v>5.5876314504173137E-3</v>
       </c>
-      <c r="AC26" s="28">
-        <f>AC24*$B$41^2</f>
+      <c r="AC27" s="28">
+        <f t="shared" si="2"/>
         <v>4.5513288756532003E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B27" s="14"/>
-      <c r="E27" s="14"/>
-    </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="14"/>
+      <c r="E28" s="14"/>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="B29" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C29" s="23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A29" s="22" t="s">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A30" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="19">
+      <c r="B30" s="19">
         <v>-9.6999999999999995E-8</v>
       </c>
-      <c r="C29" s="19">
+      <c r="C30" s="19">
         <v>4.3299999999999997E-8</v>
       </c>
-      <c r="F29" s="19">
+      <c r="F30" s="19">
         <v>-5.5100000000000002E-9</v>
       </c>
-      <c r="G29" s="19">
+      <c r="G30" s="19">
         <v>1.9799999999999999E-8</v>
       </c>
-      <c r="J29" s="19">
+      <c r="J30" s="19">
         <v>-2.6799999999999998E-8</v>
       </c>
-      <c r="K29" s="19">
+      <c r="K30" s="19">
         <v>2.11E-8</v>
       </c>
-      <c r="N29" s="19">
+      <c r="N30" s="19">
         <v>-8.72E-8</v>
       </c>
-      <c r="O29" s="19">
+      <c r="O30" s="19">
         <v>3.0400000000000001E-8</v>
       </c>
-      <c r="R29" s="19">
+      <c r="R30" s="19">
         <v>-1.1199999999999999E-8</v>
       </c>
-      <c r="S29" s="19">
+      <c r="S30" s="19">
         <v>9.5999999999999999E-9</v>
       </c>
-      <c r="V29" s="19">
+      <c r="V30" s="19">
         <v>-3.5199999999999998E-8</v>
       </c>
-      <c r="W29" s="19">
+      <c r="W30" s="19">
         <v>1.4E-8</v>
       </c>
-      <c r="Z29" s="19">
+      <c r="Z30" s="19">
         <v>-2.7599999999999999E-8</v>
       </c>
-      <c r="AA29" s="19">
+      <c r="AA30" s="19">
         <v>8.4700000000000007E-9</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A30" s="26" t="s">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A31" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="19">
+      <c r="B31" s="19">
         <v>2.0099999999999999E-9</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C31" s="19">
         <v>1.1399999999999999E-10</v>
       </c>
-      <c r="F30" s="19">
+      <c r="F31" s="19">
         <v>1.21E-9</v>
       </c>
-      <c r="G30" s="19">
+      <c r="G31" s="19">
         <v>5.2199999999999998E-11</v>
       </c>
-      <c r="J30" s="19">
+      <c r="J31" s="19">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="K30" s="19">
+      <c r="K31" s="19">
         <v>5.6599999999999997E-11</v>
       </c>
-      <c r="N30" s="19">
+      <c r="N31" s="19">
         <v>8.2199999999999995E-10</v>
       </c>
-      <c r="O30" s="19">
+      <c r="O31" s="19">
         <v>7.0099999999999996E-11</v>
       </c>
-      <c r="R30" s="19">
+      <c r="R31" s="19">
         <v>3.0299999999999999E-10</v>
       </c>
-      <c r="S30" s="19">
+      <c r="S31" s="19">
         <v>2.0999999999999999E-11</v>
       </c>
-      <c r="V30" s="19">
+      <c r="V31" s="19">
         <v>2.7399999999999998E-10</v>
       </c>
-      <c r="W30" s="19">
+      <c r="W31" s="19">
         <v>1.58E-11</v>
       </c>
-      <c r="Z30" s="19">
+      <c r="Z31" s="19">
         <v>2.0800000000000001E-10</v>
       </c>
-      <c r="AA30" s="19">
+      <c r="AA31" s="19">
         <v>6.5799999999999998E-12</v>
       </c>
     </row>
-    <row r="31" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="22" t="s">
+    <row r="32" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="19">
-        <f>B30*1000000</f>
-        <v>2.0100000000000001E-3</v>
-      </c>
-      <c r="C31" s="19">
-        <f>C30*1000000</f>
-        <v>1.1399999999999999E-4</v>
-      </c>
-      <c r="F31" s="19">
-        <f>F30*1000000</f>
-        <v>1.2099999999999999E-3</v>
-      </c>
-      <c r="G31" s="19">
-        <f>G30*1000000</f>
-        <v>5.2199999999999995E-5</v>
-      </c>
-      <c r="J31" s="19">
-        <f>J30*1000000</f>
-        <v>1E-3</v>
-      </c>
-      <c r="K31" s="19">
-        <f>K30*1000000</f>
-        <v>5.66E-5</v>
-      </c>
-      <c r="N31" s="19">
-        <f>N30*1000000</f>
-        <v>8.2199999999999992E-4</v>
-      </c>
-      <c r="O31" s="19">
-        <f>O30*1000000</f>
-        <v>7.0099999999999996E-5</v>
-      </c>
-      <c r="R31" s="19">
-        <f>R30*1000000</f>
-        <v>3.0299999999999999E-4</v>
-      </c>
-      <c r="S31" s="19">
-        <f>S30*1000000</f>
-        <v>2.0999999999999999E-5</v>
-      </c>
-      <c r="V31" s="19">
-        <f>V30*1000000</f>
-        <v>2.7399999999999999E-4</v>
-      </c>
-      <c r="W31" s="19">
-        <f>W30*1000000</f>
-        <v>1.5800000000000001E-5</v>
-      </c>
-      <c r="Z31" s="19">
-        <f>Z30*1000000</f>
-        <v>2.0800000000000001E-4</v>
-      </c>
-      <c r="AA31" s="19">
-        <f>AA30*1000000</f>
-        <v>6.5799999999999997E-6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:29" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="22" t="s">
+      <c r="B32" s="19">
+        <f>B31*1000000*0.000000001</f>
+        <v>2.0100000000000001E-12</v>
+      </c>
+      <c r="C32" s="19">
+        <f>C31*1000000*0.000000001</f>
+        <v>1.1399999999999999E-13</v>
+      </c>
+      <c r="F32" s="19">
+        <f>F31*1000000*0.000000001</f>
+        <v>1.2100000000000001E-12</v>
+      </c>
+      <c r="G32" s="19">
+        <f>G31*1000000*0.000000001</f>
+        <v>5.2200000000000001E-14</v>
+      </c>
+      <c r="J32" s="19">
+        <f>J31*1000000*0.000000001</f>
+        <v>1.0000000000000002E-12</v>
+      </c>
+      <c r="K32" s="19">
+        <f>K31*1000000*0.000000001</f>
+        <v>5.6600000000000006E-14</v>
+      </c>
+      <c r="N32" s="19">
+        <f>N31*1000000*0.000000001</f>
+        <v>8.2199999999999993E-13</v>
+      </c>
+      <c r="O32" s="19">
+        <f>O31*1000000*0.000000001</f>
+        <v>7.0099999999999999E-14</v>
+      </c>
+      <c r="R32" s="19">
+        <f>R31*1000000*0.000000001</f>
+        <v>3.0300000000000002E-13</v>
+      </c>
+      <c r="S32" s="19">
+        <f>S31*1000000*0.000000001</f>
+        <v>2.0999999999999999E-14</v>
+      </c>
+      <c r="V32" s="19">
+        <f>V31*1000000*0.000000001</f>
+        <v>2.7399999999999999E-13</v>
+      </c>
+      <c r="W32" s="19">
+        <f>W31*1000000*0.000000001</f>
+        <v>1.5800000000000003E-14</v>
+      </c>
+      <c r="Z32" s="19">
+        <f>Z31*1000000*0.000000001</f>
+        <v>2.0800000000000002E-13</v>
+      </c>
+      <c r="AA32" s="19">
+        <f>AA31*1000000*0.000000001</f>
+        <v>6.5800000000000004E-15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="28">
-        <f>B31</f>
-        <v>2.0100000000000001E-3</v>
-      </c>
-      <c r="C32" s="28">
-        <f>C31</f>
-        <v>1.1399999999999999E-4</v>
-      </c>
-      <c r="D32" s="28"/>
-      <c r="F32" s="28">
-        <f>F31</f>
-        <v>1.2099999999999999E-3</v>
-      </c>
-      <c r="G32" s="28">
-        <f>G31</f>
-        <v>5.2199999999999995E-5</v>
-      </c>
-      <c r="J32" s="28">
-        <f>J31</f>
-        <v>1E-3</v>
-      </c>
-      <c r="K32" s="28">
-        <f>K31</f>
-        <v>5.66E-5</v>
-      </c>
-      <c r="N32" s="28">
-        <f>N31</f>
-        <v>8.2199999999999992E-4</v>
-      </c>
-      <c r="O32" s="28">
-        <f>O31</f>
-        <v>7.0099999999999996E-5</v>
-      </c>
-      <c r="R32" s="28">
-        <f>R31</f>
-        <v>3.0299999999999999E-4</v>
-      </c>
-      <c r="S32" s="28">
-        <f>S31</f>
-        <v>2.0999999999999999E-5</v>
-      </c>
-      <c r="V32" s="28">
-        <f>V31</f>
-        <v>2.7399999999999999E-4</v>
-      </c>
-      <c r="W32" s="28">
-        <f>W31</f>
-        <v>1.5800000000000001E-5</v>
-      </c>
-      <c r="Z32" s="28">
-        <f>Z31</f>
-        <v>2.0800000000000001E-4</v>
-      </c>
-      <c r="AA32" s="28">
-        <f>AA31</f>
-        <v>6.5799999999999997E-6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="22"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="N33" s="19"/>
-      <c r="O33" s="19"/>
-      <c r="R33" s="19"/>
-      <c r="S33" s="19"/>
-      <c r="V33" s="19"/>
-      <c r="W33" s="19"/>
-      <c r="Z33" s="19"/>
-      <c r="AA33" s="19"/>
-    </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B34" s="22" t="s">
+      <c r="B33" s="28">
+        <f>B32</f>
+        <v>2.0100000000000001E-12</v>
+      </c>
+      <c r="C33" s="28">
+        <f>C32</f>
+        <v>1.1399999999999999E-13</v>
+      </c>
+      <c r="D33" s="28"/>
+      <c r="F33" s="28">
+        <f>F32</f>
+        <v>1.2100000000000001E-12</v>
+      </c>
+      <c r="G33" s="28">
+        <f>G32</f>
+        <v>5.2200000000000001E-14</v>
+      </c>
+      <c r="J33" s="28">
+        <f>J32</f>
+        <v>1.0000000000000002E-12</v>
+      </c>
+      <c r="K33" s="28">
+        <f>K32</f>
+        <v>5.6600000000000006E-14</v>
+      </c>
+      <c r="N33" s="28">
+        <f>N32</f>
+        <v>8.2199999999999993E-13</v>
+      </c>
+      <c r="O33" s="28">
+        <f>O32</f>
+        <v>7.0099999999999999E-14</v>
+      </c>
+      <c r="R33" s="28">
+        <f>R32</f>
+        <v>3.0300000000000002E-13</v>
+      </c>
+      <c r="S33" s="28">
+        <f>S32</f>
+        <v>2.0999999999999999E-14</v>
+      </c>
+      <c r="V33" s="28">
+        <f>V32</f>
+        <v>2.7399999999999999E-13</v>
+      </c>
+      <c r="W33" s="28">
+        <f>W32</f>
+        <v>1.5800000000000003E-14</v>
+      </c>
+      <c r="Z33" s="28">
+        <f>Z32</f>
+        <v>2.0800000000000002E-13</v>
+      </c>
+      <c r="AA33" s="28">
+        <f>AA32</f>
+        <v>6.5800000000000004E-15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="22"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="V34" s="19"/>
+      <c r="W34" s="19"/>
+      <c r="Z34" s="19"/>
+      <c r="AA34" s="19"/>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B35" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="23" t="s">
+      <c r="C35" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="19"/>
-    </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A35" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="12">
-        <v>16.25</v>
-      </c>
-      <c r="C35" s="12">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="D35" s="19"/>
-      <c r="F35">
-        <v>16.36</v>
-      </c>
-      <c r="G35">
-        <v>0.09</v>
-      </c>
-      <c r="J35">
-        <v>16.87</v>
-      </c>
-      <c r="K35">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="N35">
-        <v>17.239999999999998</v>
-      </c>
-      <c r="O35">
-        <v>0.03</v>
-      </c>
-      <c r="R35">
-        <v>17.3</v>
-      </c>
-      <c r="S35">
-        <v>0.01</v>
-      </c>
-      <c r="V35">
-        <v>17.170000000000002</v>
-      </c>
-      <c r="W35">
-        <v>0.04</v>
-      </c>
-      <c r="Z35">
-        <v>16.97</v>
-      </c>
-      <c r="AA35">
-        <v>7.0000000000000007E-2</v>
+      <c r="D35" s="19" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="12">
+        <v>16.25</v>
+      </c>
+      <c r="C36" s="12">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D36" s="19"/>
+      <c r="F36">
+        <v>16.36</v>
+      </c>
+      <c r="G36">
+        <v>0.09</v>
+      </c>
+      <c r="J36">
+        <v>16.87</v>
+      </c>
+      <c r="K36">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N36">
+        <v>17.239999999999998</v>
+      </c>
+      <c r="O36">
+        <v>0.03</v>
+      </c>
+      <c r="R36">
+        <v>17.3</v>
+      </c>
+      <c r="S36">
+        <v>0.01</v>
+      </c>
+      <c r="V36">
+        <v>17.170000000000002</v>
+      </c>
+      <c r="W36">
+        <v>0.04</v>
+      </c>
+      <c r="Z36">
+        <v>16.97</v>
+      </c>
+      <c r="AA36">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A37" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="19">
+      <c r="B37" s="19">
         <v>-4.0899999999999999E-3</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C37" s="19">
         <v>1.9699999999999999E-4</v>
-      </c>
-      <c r="D36" s="19"/>
-      <c r="F36" s="19">
-        <v>-3.62E-3</v>
-      </c>
-      <c r="G36" s="19">
-        <v>2.3599999999999999E-4</v>
-      </c>
-      <c r="J36" s="19">
-        <v>-4.0600000000000002E-3</v>
-      </c>
-      <c r="K36" s="19">
-        <v>1.95E-4</v>
-      </c>
-      <c r="N36" s="19">
-        <v>-3.7599999999999999E-3</v>
-      </c>
-      <c r="O36" s="19">
-        <v>6.9800000000000003E-5</v>
-      </c>
-      <c r="R36" s="19">
-        <v>-2.5799999999999998E-3</v>
-      </c>
-      <c r="S36" s="19">
-        <v>3.2700000000000002E-5</v>
-      </c>
-      <c r="V36" s="19">
-        <v>-1.66E-3</v>
-      </c>
-      <c r="W36" s="19">
-        <v>4.21E-5</v>
-      </c>
-      <c r="Z36" s="19">
-        <v>-1.1100000000000001E-3</v>
-      </c>
-      <c r="AA36" s="19">
-        <v>5.7500000000000002E-5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="19">
-        <f>B36*1000000</f>
-        <v>-4090</v>
-      </c>
-      <c r="C37" s="19">
-        <f>C36*1000000</f>
-        <v>197</v>
       </c>
       <c r="D37" s="19"/>
       <c r="F37" s="19">
-        <f>F36*1000000</f>
+        <v>-3.62E-3</v>
+      </c>
+      <c r="G37" s="19">
+        <v>2.3599999999999999E-4</v>
+      </c>
+      <c r="J37" s="19">
+        <v>-4.0600000000000002E-3</v>
+      </c>
+      <c r="K37" s="19">
+        <v>1.95E-4</v>
+      </c>
+      <c r="N37" s="19">
+        <v>-3.7599999999999999E-3</v>
+      </c>
+      <c r="O37" s="19">
+        <v>6.9800000000000003E-5</v>
+      </c>
+      <c r="R37" s="19">
+        <v>-2.5799999999999998E-3</v>
+      </c>
+      <c r="S37" s="19">
+        <v>3.2700000000000002E-5</v>
+      </c>
+      <c r="V37" s="19">
+        <v>-1.66E-3</v>
+      </c>
+      <c r="W37" s="19">
+        <v>4.21E-5</v>
+      </c>
+      <c r="Z37" s="19">
+        <v>-1.1100000000000001E-3</v>
+      </c>
+      <c r="AA37" s="19">
+        <v>5.7500000000000002E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="19">
+        <f>B37*1000000</f>
+        <v>-4090</v>
+      </c>
+      <c r="C38" s="19">
+        <f>C37*1000000</f>
+        <v>197</v>
+      </c>
+      <c r="D38" s="19"/>
+      <c r="F38" s="19">
+        <f>F37*1000000</f>
         <v>-3620</v>
       </c>
-      <c r="G37" s="19">
-        <f>G36*1000000</f>
+      <c r="G38" s="19">
+        <f>G37*1000000</f>
         <v>236</v>
       </c>
-      <c r="J37" s="19">
-        <f>J36*1000000</f>
+      <c r="J38" s="19">
+        <f>J37*1000000</f>
         <v>-4060.0000000000005</v>
       </c>
-      <c r="K37" s="19">
-        <f>K36*1000000</f>
+      <c r="K38" s="19">
+        <f>K37*1000000</f>
         <v>195</v>
       </c>
-      <c r="N37" s="19">
-        <f>N36*1000000</f>
+      <c r="N38" s="19">
+        <f>N37*1000000</f>
         <v>-3760</v>
       </c>
-      <c r="O37" s="19">
-        <f>O36*1000000</f>
+      <c r="O38" s="19">
+        <f>O37*1000000</f>
         <v>69.8</v>
       </c>
-      <c r="R37" s="19">
-        <f>R36*1000000</f>
+      <c r="R38" s="19">
+        <f>R37*1000000</f>
         <v>-2580</v>
       </c>
-      <c r="S37" s="19">
-        <f>S36*1000000</f>
+      <c r="S38" s="19">
+        <f>S37*1000000</f>
         <v>32.700000000000003</v>
       </c>
-      <c r="V37" s="19">
-        <f>V36*1000000</f>
+      <c r="V38" s="19">
+        <f>V37*1000000</f>
         <v>-1660</v>
       </c>
-      <c r="W37" s="19">
-        <f>W36*1000000</f>
+      <c r="W38" s="19">
+        <f>W37*1000000</f>
         <v>42.1</v>
       </c>
-      <c r="Z37" s="19">
-        <f>Z36*1000000</f>
+      <c r="Z38" s="19">
+        <f>Z37*1000000</f>
         <v>-1110</v>
       </c>
-      <c r="AA37" s="19">
-        <f>AA36*1000000</f>
+      <c r="AA38" s="19">
+        <f>AA37*1000000</f>
         <v>57.5</v>
       </c>
     </row>
-    <row r="38" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="22" t="s">
+    <row r="39" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="28">
-        <f>-B37*$B$41^2</f>
+      <c r="B39" s="28">
+        <f>-B38*$B$42^2</f>
         <v>5.7276723388989502E-2</v>
       </c>
-      <c r="C38" s="28">
-        <f>C37*$B$41^2</f>
+      <c r="C39" s="28">
+        <f>C38*$B$42^2</f>
         <v>2.7588055030882477E-3</v>
       </c>
-      <c r="D38" s="28"/>
-      <c r="F38" s="28">
-        <f>-F37*$B$41^2</f>
+      <c r="D39" s="28"/>
+      <c r="F39" s="28">
+        <f>-F38*$B$42^2</f>
         <v>5.0694801630352566E-2</v>
       </c>
-      <c r="G38" s="28">
-        <f>G37*$B$41^2</f>
+      <c r="G39" s="28">
+        <f>G38*$B$42^2</f>
         <v>3.3049649681666316E-3</v>
       </c>
-      <c r="J38" s="28">
-        <f>-J37*$B$41^2</f>
+      <c r="J39" s="28">
+        <f>-J38*$B$42^2</f>
         <v>5.6856600723544599E-2</v>
       </c>
-      <c r="K38" s="28">
-        <f>K37*$B$41^2</f>
+      <c r="K39" s="28">
+        <f>K38*$B$42^2</f>
         <v>2.7307973253919201E-3</v>
       </c>
-      <c r="N38" s="28">
-        <f>-N37*$B$41^2</f>
+      <c r="N39" s="28">
+        <f>-N38*$B$42^2</f>
         <v>5.2655374069095484E-2</v>
       </c>
-      <c r="O38" s="28">
-        <f>O37*$B$41^2</f>
+      <c r="O39" s="28">
+        <f>O38*$B$42^2</f>
         <v>9.7748540160182574E-4</v>
       </c>
-      <c r="R38" s="28">
-        <f>-R37*$B$41^2</f>
+      <c r="R39" s="28">
+        <f>-R38*$B$42^2</f>
         <v>3.6130549228262331E-2</v>
       </c>
-      <c r="S38" s="28">
-        <f>S37*$B$41^2</f>
+      <c r="S39" s="28">
+        <f>S38*$B$42^2</f>
         <v>4.5793370533495282E-4</v>
       </c>
-      <c r="V38" s="28">
-        <f>-V37*$B$41^2</f>
+      <c r="V39" s="28">
+        <f>-V38*$B$42^2</f>
         <v>2.3246787487951729E-2</v>
       </c>
-      <c r="W38" s="28">
-        <f>W37*$B$41^2</f>
+      <c r="W39" s="28">
+        <f>W38*$B$42^2</f>
         <v>5.8957214050769154E-4</v>
       </c>
-      <c r="Z38" s="28">
-        <f>-Z37*$B$41^2</f>
+      <c r="Z39" s="28">
+        <f>-Z38*$B$42^2</f>
         <v>1.55445386214617E-2</v>
       </c>
-      <c r="AA38" s="28">
-        <f>AA37*$B$41^2</f>
+      <c r="AA39" s="28">
+        <f>AA38*$B$42^2</f>
         <v>8.0523510876941238E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="D39" s="19"/>
-    </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A40" s="22" t="s">
+      <c r="D40" s="19"/>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A41" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B40" s="12">
+      <c r="B41" s="12">
         <f>0.009</f>
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="D40" s="19"/>
-    </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A41" s="22" t="s">
+      <c r="D41" s="19"/>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A42" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="12">
-        <f>B40/2.405</f>
+      <c r="B42" s="12">
+        <f>B41/2.405</f>
         <v>3.7422037422037424E-3</v>
       </c>
-      <c r="D41" s="19"/>
-    </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
       <c r="D42" s="19"/>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.3">
       <c r="D43" s="19"/>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A44" s="12" t="s">
+      <c r="D44" s="19"/>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A45" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="33" t="s">
+      <c r="B45" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C44" s="33"/>
-      <c r="D44" s="34" t="s">
+      <c r="C45" s="34"/>
+      <c r="D45" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E44" s="34"/>
-      <c r="F44" s="33" t="s">
+      <c r="E45" s="35"/>
+      <c r="F45" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="G44" s="33"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33" t="s">
+      <c r="G45" s="34"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="K44" s="33"/>
-      <c r="L44" s="33"/>
-      <c r="M44" s="33"/>
-      <c r="N44" s="14" t="s">
+      <c r="K45" s="34"/>
+      <c r="L45" s="34"/>
+      <c r="M45" s="34"/>
+      <c r="N45" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="O44" s="33" t="s">
+      <c r="O45" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="P44" s="33"/>
-      <c r="Q44" s="34" t="s">
+      <c r="P45" s="34"/>
+      <c r="Q45" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="R44" s="34"/>
-      <c r="S44" s="33" t="s">
+      <c r="R45" s="35"/>
+      <c r="S45" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="T44" s="33"/>
-      <c r="U44" s="33"/>
-      <c r="V44" s="33"/>
-      <c r="W44" s="33" t="s">
+      <c r="T45" s="34"/>
+      <c r="U45" s="34"/>
+      <c r="V45" s="34"/>
+      <c r="W45" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="X44" s="33"/>
-      <c r="Y44" s="33"/>
-      <c r="Z44" s="33"/>
-    </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B45" s="12" t="s">
+      <c r="X45" s="34"/>
+      <c r="Y45" s="34"/>
+      <c r="Z45" s="34"/>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B46" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C45" s="12" t="s">
+      <c r="C46" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D46" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E46" t="s">
         <v>30</v>
       </c>
-      <c r="F45" s="14" t="s">
+      <c r="F46" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G45" s="14" t="s">
+      <c r="G46" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H45" s="14" t="s">
+      <c r="H46" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="I45" s="14" t="s">
+      <c r="I46" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="J45" s="14" t="s">
+      <c r="J46" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="K45" s="14" t="s">
+      <c r="K46" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="L45" s="14" t="s">
+      <c r="L46" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="M45" s="14" t="s">
+      <c r="M46" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="N45" s="14" t="s">
+      <c r="N46" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="O45" s="14" t="s">
+      <c r="O46" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="P45" s="14" t="s">
+      <c r="P46" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="Q45" s="14" t="s">
+      <c r="Q46" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="R45" s="14" t="s">
+      <c r="R46" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="S45" s="14" t="s">
+      <c r="S46" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="T45" s="14" t="s">
+      <c r="T46" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="U45" s="14" t="s">
+      <c r="U46" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="V45" s="14" t="s">
+      <c r="V46" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="W45" s="14" t="s">
+      <c r="W46" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="X45" s="14" t="s">
+      <c r="X46" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="Y45" s="14" t="s">
+      <c r="Y46" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="Z45" s="14" t="s">
+      <c r="Z46" s="14" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A46" s="12">
-        <v>5</v>
-      </c>
-      <c r="B46" s="19">
-        <f>B32</f>
-        <v>2.0100000000000001E-3</v>
-      </c>
-      <c r="C46" s="29">
-        <f>C32</f>
-        <v>1.1399999999999999E-4</v>
-      </c>
-      <c r="D46" s="19">
-        <f>B38</f>
-        <v>5.7276723388989502E-2</v>
-      </c>
-      <c r="E46" s="29">
-        <f>C38</f>
-        <v>2.7588055030882477E-3</v>
-      </c>
-      <c r="F46" s="19">
-        <f>B25</f>
-        <v>7.7343000000000008E-4</v>
-      </c>
-      <c r="G46" s="29">
-        <f>C25</f>
-        <v>4.0171000000000002E-7</v>
-      </c>
-      <c r="H46" s="19">
-        <f>B26</f>
-        <v>2.84283003617723E-2</v>
-      </c>
-      <c r="I46" s="29">
-        <f>C26</f>
-        <v>4.0471816771193075E-4</v>
-      </c>
-      <c r="J46" s="19">
-        <f>D25</f>
-        <v>6.7499999999999993E-4</v>
-      </c>
-      <c r="K46" s="19">
-        <f>E25</f>
-        <v>2.2615999999999997E-6</v>
-      </c>
-      <c r="L46" s="19">
-        <f>D26</f>
-        <v>3.1509199908368313E-2</v>
-      </c>
-      <c r="M46" s="19">
-        <f>E26</f>
-        <v>1.232359818638405E-3</v>
-      </c>
-      <c r="N46" s="14">
-        <v>5</v>
-      </c>
-      <c r="O46" s="30">
-        <f>B46*1000</f>
-        <v>2.0100000000000002</v>
-      </c>
-      <c r="P46" s="30">
-        <f>C46*1000</f>
-        <v>0.11399999999999999</v>
-      </c>
-      <c r="Q46" s="32">
-        <f>D46*1000</f>
-        <v>57.276723388989502</v>
-      </c>
-      <c r="R46" s="32">
-        <f>E46*1000</f>
-        <v>2.7588055030882477</v>
-      </c>
-      <c r="S46" s="25">
-        <f>F46*1000</f>
-        <v>0.77343000000000006</v>
-      </c>
-      <c r="T46" s="25">
-        <f>G46*1000</f>
-        <v>4.0171E-4</v>
-      </c>
-      <c r="U46" s="32">
-        <f>H46*1000</f>
-        <v>28.428300361772301</v>
-      </c>
-      <c r="V46" s="32">
-        <f>I46*1000</f>
-        <v>0.40471816771193075</v>
-      </c>
-      <c r="W46" s="25">
-        <f>J46*1000</f>
-        <v>0.67499999999999993</v>
-      </c>
-      <c r="X46" s="25">
-        <f>K46*1000</f>
-        <v>2.2615999999999995E-3</v>
-      </c>
-      <c r="Y46" s="32">
-        <f>L46*1000</f>
-        <v>31.509199908368313</v>
-      </c>
-      <c r="Z46" s="32">
-        <f>M46*1000</f>
-        <v>1.232359818638405</v>
       </c>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A47" s="12">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B47" s="19">
-        <f>F32</f>
-        <v>1.2099999999999999E-3</v>
+        <f>B33</f>
+        <v>2.0100000000000001E-12</v>
       </c>
       <c r="C47" s="29">
-        <f>G32</f>
-        <v>5.2199999999999995E-5</v>
+        <f>C33</f>
+        <v>1.1399999999999999E-13</v>
       </c>
       <c r="D47" s="19">
-        <f>F38</f>
-        <v>5.0694801630352566E-2</v>
+        <f>B39</f>
+        <v>5.7276723388989502E-2</v>
       </c>
       <c r="E47" s="29">
-        <f>G38</f>
-        <v>3.3049649681666316E-3</v>
+        <f>C39</f>
+        <v>2.7588055030882477E-3</v>
       </c>
       <c r="F47" s="19">
-        <f>F25</f>
-        <v>5.7563999999999998E-4</v>
+        <f>B26</f>
+        <v>7.7343000000000017E-13</v>
       </c>
       <c r="G47" s="29">
-        <f>G25</f>
-        <v>5.502E-6</v>
+        <f>C26</f>
+        <v>4.0171000000000007E-16</v>
       </c>
       <c r="H47" s="19">
-        <f>F26</f>
-        <v>2.1846378603135361E-2</v>
+        <f>B27</f>
+        <v>2.84283003617723E-2</v>
       </c>
       <c r="I47" s="29">
-        <f>G26</f>
-        <v>1.4704293290571878E-3</v>
+        <f>C27</f>
+        <v>4.0471816771193075E-4</v>
       </c>
       <c r="J47" s="19">
-        <f>H25</f>
-        <v>6.4185999999999996E-4</v>
+        <f>D26</f>
+        <v>6.7499999999999995E-13</v>
       </c>
       <c r="K47" s="19">
-        <f>I25</f>
-        <v>1.1745E-5</v>
+        <f>E26</f>
+        <v>2.2615999999999999E-15</v>
       </c>
       <c r="L47" s="19">
-        <f>H26</f>
-        <v>1.8765479056539348E-2</v>
+        <f>D27</f>
+        <v>3.1509199908368313E-2</v>
       </c>
       <c r="M47" s="19">
-        <f>I26</f>
-        <v>2.0305928829837355E-3</v>
+        <f>E27</f>
+        <v>1.232359818638405E-3</v>
       </c>
       <c r="N47" s="14">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="O47" s="30">
-        <f>B47*1000</f>
-        <v>1.21</v>
+        <f t="shared" ref="O47:Z53" si="3">B47*1000</f>
+        <v>2.0100000000000003E-9</v>
       </c>
       <c r="P47" s="30">
-        <f>C47*1000</f>
-        <v>5.2199999999999996E-2</v>
+        <f t="shared" si="3"/>
+        <v>1.1399999999999999E-10</v>
       </c>
       <c r="Q47" s="32">
-        <f>D47*1000</f>
-        <v>50.694801630352565</v>
+        <f t="shared" si="3"/>
+        <v>57.276723388989502</v>
       </c>
       <c r="R47" s="32">
-        <f>E47*1000</f>
-        <v>3.3049649681666318</v>
-      </c>
-      <c r="S47" s="31">
-        <f>F47*1000</f>
-        <v>0.57563999999999993</v>
-      </c>
-      <c r="T47" s="31">
-        <f>G47*1000</f>
-        <v>5.5019999999999999E-3</v>
+        <f t="shared" si="3"/>
+        <v>2.7588055030882477</v>
+      </c>
+      <c r="S47" s="25">
+        <f t="shared" si="3"/>
+        <v>7.7343000000000019E-10</v>
+      </c>
+      <c r="T47" s="25">
+        <f t="shared" si="3"/>
+        <v>4.0171000000000006E-13</v>
       </c>
       <c r="U47" s="32">
-        <f>H47*1000</f>
-        <v>21.84637860313536</v>
+        <f t="shared" si="3"/>
+        <v>28.428300361772301</v>
       </c>
       <c r="V47" s="32">
-        <f>I47*1000</f>
-        <v>1.4704293290571879</v>
-      </c>
-      <c r="W47" s="31">
-        <f>J47*1000</f>
-        <v>0.64185999999999999</v>
-      </c>
-      <c r="X47" s="31">
-        <f>K47*1000</f>
-        <v>1.1745E-2</v>
+        <f t="shared" si="3"/>
+        <v>0.40471816771193075</v>
+      </c>
+      <c r="W47" s="25">
+        <f t="shared" si="3"/>
+        <v>6.7499999999999994E-10</v>
+      </c>
+      <c r="X47" s="25">
+        <f t="shared" si="3"/>
+        <v>2.2616E-12</v>
       </c>
       <c r="Y47" s="32">
-        <f>L47*1000</f>
-        <v>18.765479056539348</v>
+        <f t="shared" si="3"/>
+        <v>31.509199908368313</v>
       </c>
       <c r="Z47" s="32">
-        <f>M47*1000</f>
-        <v>2.0305928829837354</v>
+        <f t="shared" si="3"/>
+        <v>1.232359818638405</v>
       </c>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A48" s="12">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B48" s="19">
-        <f>J32</f>
-        <v>1E-3</v>
+        <f>F33</f>
+        <v>1.2100000000000001E-12</v>
       </c>
       <c r="C48" s="29">
-        <f>K32</f>
-        <v>5.66E-5</v>
+        <f>G33</f>
+        <v>5.2200000000000001E-14</v>
       </c>
       <c r="D48" s="19">
-        <f>J38</f>
-        <v>5.6856600723544599E-2</v>
+        <f>F39</f>
+        <v>5.0694801630352566E-2</v>
       </c>
       <c r="E48" s="29">
-        <f>K38</f>
-        <v>2.7307973253919201E-3</v>
+        <f>G39</f>
+        <v>3.3049649681666316E-3</v>
       </c>
       <c r="F48" s="19">
-        <f>J25</f>
-        <v>4.3560000000000002E-4</v>
+        <f>F26</f>
+        <v>5.7563999999999996E-13</v>
       </c>
       <c r="G48" s="29">
-        <f>K25</f>
-        <v>2.7491999999999999E-6</v>
+        <f>G26</f>
+        <v>5.5020000000000007E-15</v>
       </c>
       <c r="H48" s="19">
-        <f>J26</f>
-        <v>2.5207359926694647E-2</v>
+        <f>F27</f>
+        <v>2.1846378603135361E-2</v>
       </c>
       <c r="I48" s="29">
-        <f>K26</f>
-        <v>1.327587622805918E-3</v>
+        <f>G27</f>
+        <v>1.4704293290571878E-3</v>
       </c>
       <c r="J48" s="19">
-        <f>L25</f>
-        <v>2.7776E-4</v>
+        <f>H26</f>
+        <v>6.3106000000000014E-13</v>
       </c>
       <c r="K48" s="19">
-        <f>M25</f>
-        <v>5.2920000000000003E-6</v>
+        <f>I26</f>
+        <v>6.4963999999999996E-15</v>
       </c>
       <c r="L48" s="19">
-        <f>L26</f>
-        <v>3.4730140343445959E-2</v>
+        <f>H27</f>
+        <v>1.9465683498947534E-2</v>
       </c>
       <c r="M48" s="19">
-        <f>M26</f>
-        <v>3.0248831912033577E-3</v>
+        <f>I27</f>
+        <v>1.5264456844498425E-3</v>
       </c>
       <c r="N48" s="14">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="O48" s="30">
-        <f>B48*1000</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>1.2100000000000002E-9</v>
       </c>
       <c r="P48" s="30">
-        <f>C48*1000</f>
-        <v>5.6599999999999998E-2</v>
+        <f t="shared" si="3"/>
+        <v>5.2199999999999998E-11</v>
       </c>
       <c r="Q48" s="32">
-        <f>D48*1000</f>
-        <v>56.856600723544602</v>
+        <f t="shared" si="3"/>
+        <v>50.694801630352565</v>
       </c>
       <c r="R48" s="32">
-        <f>E48*1000</f>
-        <v>2.73079732539192</v>
+        <f t="shared" si="3"/>
+        <v>3.3049649681666318</v>
       </c>
       <c r="S48" s="31">
-        <f>F48*1000</f>
-        <v>0.43560000000000004</v>
+        <f t="shared" si="3"/>
+        <v>5.7563999999999999E-10</v>
       </c>
       <c r="T48" s="31">
-        <f>G48*1000</f>
-        <v>2.7491999999999998E-3</v>
+        <f t="shared" si="3"/>
+        <v>5.5020000000000006E-12</v>
       </c>
       <c r="U48" s="32">
-        <f>H48*1000</f>
-        <v>25.207359926694647</v>
+        <f t="shared" si="3"/>
+        <v>21.84637860313536</v>
       </c>
       <c r="V48" s="32">
-        <f>I48*1000</f>
-        <v>1.327587622805918</v>
+        <f t="shared" si="3"/>
+        <v>1.4704293290571879</v>
       </c>
       <c r="W48" s="31">
-        <f>J48*1000</f>
-        <v>0.27776000000000001</v>
+        <f t="shared" si="3"/>
+        <v>6.3106000000000009E-10</v>
       </c>
       <c r="X48" s="31">
-        <f>K48*1000</f>
-        <v>5.2920000000000007E-3</v>
+        <f t="shared" si="3"/>
+        <v>6.4963999999999997E-12</v>
       </c>
       <c r="Y48" s="32">
-        <f>L48*1000</f>
-        <v>34.73014034344596</v>
+        <f t="shared" si="3"/>
+        <v>19.465683498947534</v>
       </c>
       <c r="Z48" s="32">
-        <f>M48*1000</f>
-        <v>3.0248831912033576</v>
+        <f t="shared" si="3"/>
+        <v>1.5264456844498424</v>
       </c>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A49" s="12">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="B49" s="19">
-        <f>N32</f>
-        <v>8.2199999999999992E-4</v>
+        <f>J33</f>
+        <v>1.0000000000000002E-12</v>
       </c>
       <c r="C49" s="29">
-        <f>O32</f>
-        <v>7.0099999999999996E-5</v>
+        <f>K33</f>
+        <v>5.6600000000000006E-14</v>
       </c>
       <c r="D49" s="19">
-        <f>N38</f>
-        <v>5.2655374069095484E-2</v>
+        <f>J39</f>
+        <v>5.6856600723544599E-2</v>
       </c>
       <c r="E49" s="29">
-        <f>O38</f>
-        <v>9.7748540160182574E-4</v>
+        <f>K39</f>
+        <v>2.7307973253919201E-3</v>
       </c>
       <c r="F49" s="19">
-        <f>N25</f>
-        <v>1.8046499999999999E-4</v>
+        <f>J26</f>
+        <v>4.3560000000000008E-13</v>
       </c>
       <c r="G49" s="29">
-        <f>O25</f>
-        <v>2.9230000000000002E-6</v>
+        <f>K26</f>
+        <v>2.7492000000000002E-15</v>
       </c>
       <c r="H49" s="19">
-        <f>N26</f>
-        <v>3.7110835447633786E-2</v>
+        <f>J27</f>
+        <v>2.5207359926694647E-2</v>
       </c>
       <c r="I49" s="29">
-        <f>O26</f>
-        <v>2.2126460380098635E-3</v>
+        <f>K27</f>
+        <v>1.327587622805918E-3</v>
       </c>
       <c r="J49" s="19">
-        <f>P25</f>
-        <v>8.6939999999999991E-5</v>
+        <f>L26</f>
+        <v>2.7775999999999997E-13</v>
       </c>
       <c r="K49" s="19">
-        <f>Q25</f>
-        <v>4.9341599999999992E-7</v>
+        <f>M26</f>
+        <v>5.2920000000000008E-15</v>
       </c>
       <c r="L49" s="19">
-        <f>P26</f>
-        <v>4.4112879871715631E-2</v>
+        <f>L27</f>
+        <v>3.4730140343445959E-2</v>
       </c>
       <c r="M49" s="19">
-        <f>Q26</f>
-        <v>1.3710002982352254E-3</v>
+        <f>M27</f>
+        <v>3.0248831912033577E-3</v>
       </c>
       <c r="N49" s="14">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O49" s="30">
-        <f>B49*1000</f>
-        <v>0.82199999999999995</v>
+        <f t="shared" si="3"/>
+        <v>1.0000000000000003E-9</v>
       </c>
       <c r="P49" s="30">
-        <f>C49*1000</f>
-        <v>7.0099999999999996E-2</v>
+        <f t="shared" si="3"/>
+        <v>5.6600000000000004E-11</v>
       </c>
       <c r="Q49" s="32">
-        <f>D49*1000</f>
-        <v>52.655374069095487</v>
+        <f t="shared" si="3"/>
+        <v>56.856600723544602</v>
       </c>
       <c r="R49" s="32">
-        <f>E49*1000</f>
-        <v>0.97748540160182573</v>
+        <f t="shared" si="3"/>
+        <v>2.73079732539192</v>
       </c>
       <c r="S49" s="31">
-        <f>F49*1000</f>
-        <v>0.18046499999999999</v>
+        <f t="shared" si="3"/>
+        <v>4.3560000000000008E-10</v>
       </c>
       <c r="T49" s="31">
-        <f>G49*1000</f>
-        <v>2.9230000000000003E-3</v>
+        <f t="shared" si="3"/>
+        <v>2.7492E-12</v>
       </c>
       <c r="U49" s="32">
-        <f>H49*1000</f>
-        <v>37.110835447633789</v>
+        <f t="shared" si="3"/>
+        <v>25.207359926694647</v>
       </c>
       <c r="V49" s="32">
-        <f>I49*1000</f>
-        <v>2.2126460380098636</v>
+        <f t="shared" si="3"/>
+        <v>1.327587622805918</v>
       </c>
       <c r="W49" s="31">
-        <f>J49*1000</f>
-        <v>8.693999999999999E-2</v>
-      </c>
-      <c r="X49" s="25">
-        <f>K49*1000</f>
-        <v>4.9341599999999989E-4</v>
+        <f t="shared" si="3"/>
+        <v>2.7775999999999998E-10</v>
+      </c>
+      <c r="X49" s="31">
+        <f t="shared" si="3"/>
+        <v>5.2920000000000005E-12</v>
       </c>
       <c r="Y49" s="32">
-        <f>L49*1000</f>
-        <v>44.112879871715634</v>
+        <f t="shared" si="3"/>
+        <v>34.73014034344596</v>
       </c>
       <c r="Z49" s="32">
-        <f>M49*1000</f>
-        <v>1.3710002982352254</v>
+        <f t="shared" si="3"/>
+        <v>3.0248831912033576</v>
       </c>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A50" s="12">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B50" s="19">
-        <f>R32</f>
-        <v>3.0299999999999999E-4</v>
+        <f>N33</f>
+        <v>8.2199999999999993E-13</v>
       </c>
       <c r="C50" s="29">
-        <f>S32</f>
-        <v>2.0999999999999999E-5</v>
+        <f>O33</f>
+        <v>7.0099999999999999E-14</v>
       </c>
       <c r="D50" s="19">
-        <f>R38</f>
-        <v>3.6130549228262331E-2</v>
+        <f>N39</f>
+        <v>5.2655374069095484E-2</v>
       </c>
       <c r="E50" s="29">
-        <f>S38</f>
-        <v>4.5793370533495282E-4</v>
+        <f>O39</f>
+        <v>9.7748540160182574E-4</v>
       </c>
       <c r="F50" s="19">
-        <f>R25</f>
-        <v>2.9153999999999999E-5</v>
+        <f>N26</f>
+        <v>1.80465E-13</v>
       </c>
       <c r="G50" s="29">
-        <f>S25</f>
-        <v>1.76358E-7</v>
+        <f>O26</f>
+        <v>2.9230000000000004E-15</v>
       </c>
       <c r="H50" s="19">
-        <f>R26</f>
-        <v>3.1649240796849949E-2</v>
+        <f>N27</f>
+        <v>3.7110835447633786E-2</v>
       </c>
       <c r="I50" s="29">
-        <f>S26</f>
-        <v>7.6462325110973769E-4</v>
+        <f>O27</f>
+        <v>2.2126460380098635E-3</v>
       </c>
       <c r="J50" s="19">
-        <f>T25</f>
-        <v>4.0850000000000004E-5</v>
+        <f>P26</f>
+        <v>8.6940000000000006E-14</v>
       </c>
       <c r="K50" s="19">
-        <f>U25</f>
-        <v>1.0647000000000001E-7</v>
+        <f>Q26</f>
+        <v>4.9341599999999997E-16</v>
       </c>
       <c r="L50" s="19">
-        <f>T26</f>
-        <v>3.0108791023551941E-2</v>
+        <f>P27</f>
+        <v>4.4112879871715631E-2</v>
       </c>
       <c r="M50" s="19">
-        <f>U26</f>
-        <v>6.3718604259144804E-4</v>
+        <f>Q27</f>
+        <v>1.3710002982352254E-3</v>
       </c>
       <c r="N50" s="14">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O50" s="30">
-        <f>B50*1000</f>
-        <v>0.30299999999999999</v>
+        <f t="shared" si="3"/>
+        <v>8.2199999999999995E-10</v>
       </c>
       <c r="P50" s="30">
-        <f>C50*1000</f>
-        <v>2.0999999999999998E-2</v>
+        <f t="shared" si="3"/>
+        <v>7.0099999999999996E-11</v>
       </c>
       <c r="Q50" s="32">
-        <f>D50*1000</f>
-        <v>36.130549228262332</v>
+        <f t="shared" si="3"/>
+        <v>52.655374069095487</v>
       </c>
       <c r="R50" s="32">
-        <f>E50*1000</f>
-        <v>0.45793370533495281</v>
-      </c>
-      <c r="S50" s="25">
-        <f>F50*1000</f>
-        <v>2.9153999999999999E-2</v>
-      </c>
-      <c r="T50" s="25">
-        <f>G50*1000</f>
-        <v>1.7635799999999999E-4</v>
+        <f t="shared" si="3"/>
+        <v>0.97748540160182573</v>
+      </c>
+      <c r="S50" s="31">
+        <f t="shared" si="3"/>
+        <v>1.8046500000000001E-10</v>
+      </c>
+      <c r="T50" s="31">
+        <f t="shared" si="3"/>
+        <v>2.9230000000000004E-12</v>
       </c>
       <c r="U50" s="32">
-        <f>H50*1000</f>
-        <v>31.649240796849949</v>
+        <f t="shared" si="3"/>
+        <v>37.110835447633789</v>
       </c>
       <c r="V50" s="32">
-        <f>I50*1000</f>
-        <v>0.76462325110973772</v>
-      </c>
-      <c r="W50" s="25">
-        <f>J50*1000</f>
-        <v>4.0850000000000004E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.2126460380098636</v>
+      </c>
+      <c r="W50" s="31">
+        <f t="shared" si="3"/>
+        <v>8.6940000000000012E-11</v>
       </c>
       <c r="X50" s="25">
-        <f>K50*1000</f>
-        <v>1.0647000000000002E-4</v>
+        <f t="shared" si="3"/>
+        <v>4.9341599999999994E-13</v>
       </c>
       <c r="Y50" s="32">
-        <f>L50*1000</f>
-        <v>30.108791023551941</v>
+        <f t="shared" si="3"/>
+        <v>44.112879871715634</v>
       </c>
       <c r="Z50" s="32">
-        <f>M50*1000</f>
-        <v>0.63718604259144807</v>
+        <f t="shared" si="3"/>
+        <v>1.3710002982352254</v>
       </c>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A51" s="12">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="B51" s="19">
-        <f>V32</f>
-        <v>2.7399999999999999E-4</v>
+        <f>R33</f>
+        <v>3.0300000000000002E-13</v>
       </c>
       <c r="C51" s="29">
-        <f>W32</f>
-        <v>1.5800000000000001E-5</v>
+        <f>S33</f>
+        <v>2.0999999999999999E-14</v>
       </c>
       <c r="D51" s="19">
-        <f>V38</f>
-        <v>2.3246787487951729E-2</v>
+        <f>R39</f>
+        <v>3.6130549228262331E-2</v>
       </c>
       <c r="E51" s="29">
-        <f>W38</f>
-        <v>5.8957214050769154E-4</v>
+        <f>S39</f>
+        <v>4.5793370533495282E-4</v>
       </c>
       <c r="F51" s="19">
-        <f>V25</f>
-        <v>5.9039999999999997E-5</v>
+        <f>R26</f>
+        <v>2.9154E-14</v>
       </c>
       <c r="G51" s="29">
-        <f>W25</f>
-        <v>4.3871199999999994E-7</v>
+        <f>S26</f>
+        <v>1.7635800000000001E-16</v>
       </c>
       <c r="H51" s="19">
-        <f>V26</f>
-        <v>1.680490661779643E-2</v>
+        <f>R27</f>
+        <v>3.1649240796849949E-2</v>
       </c>
       <c r="I51" s="29">
-        <f>W26</f>
-        <v>6.8339953579038819E-4</v>
+        <f>S27</f>
+        <v>7.6462325110973769E-4</v>
       </c>
       <c r="J51" s="19">
-        <f>X25</f>
-        <v>6.8627999999999994E-5</v>
+        <f>T26</f>
+        <v>4.085000000000001E-14</v>
       </c>
       <c r="K51" s="19">
-        <f>Y25</f>
-        <v>2.41042E-7</v>
+        <f>U26</f>
+        <v>1.0647000000000001E-16</v>
       </c>
       <c r="L51" s="19">
-        <f>X26</f>
-        <v>1.5964661286906611E-2</v>
+        <f>T27</f>
+        <v>3.0108791023551941E-2</v>
       </c>
       <c r="M51" s="19">
-        <f>Y26</f>
-        <v>5.3495619399985313E-4</v>
+        <f>U27</f>
+        <v>6.3718604259144804E-4</v>
       </c>
       <c r="N51" s="14">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="O51" s="30">
-        <f>B51*1000</f>
-        <v>0.27399999999999997</v>
+        <f t="shared" si="3"/>
+        <v>3.0300000000000004E-10</v>
       </c>
       <c r="P51" s="30">
-        <f>C51*1000</f>
-        <v>1.5800000000000002E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.0999999999999999E-11</v>
       </c>
       <c r="Q51" s="32">
-        <f>D51*1000</f>
-        <v>23.246787487951728</v>
+        <f t="shared" si="3"/>
+        <v>36.130549228262332</v>
       </c>
       <c r="R51" s="32">
-        <f>E51*1000</f>
-        <v>0.58957214050769158</v>
+        <f t="shared" si="3"/>
+        <v>0.45793370533495281</v>
       </c>
       <c r="S51" s="25">
-        <f>F51*1000</f>
-        <v>5.9039999999999995E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.9154E-11</v>
       </c>
       <c r="T51" s="25">
-        <f>G51*1000</f>
-        <v>4.3871199999999996E-4</v>
+        <f t="shared" si="3"/>
+        <v>1.76358E-13</v>
       </c>
       <c r="U51" s="32">
-        <f>H51*1000</f>
-        <v>16.80490661779643</v>
+        <f t="shared" si="3"/>
+        <v>31.649240796849949</v>
       </c>
       <c r="V51" s="32">
-        <f>I51*1000</f>
-        <v>0.68339953579038815</v>
+        <f t="shared" si="3"/>
+        <v>0.76462325110973772</v>
       </c>
       <c r="W51" s="25">
-        <f>J51*1000</f>
-        <v>6.8627999999999995E-2</v>
+        <f t="shared" si="3"/>
+        <v>4.0850000000000013E-11</v>
       </c>
       <c r="X51" s="25">
-        <f>K51*1000</f>
-        <v>2.4104199999999999E-4</v>
+        <f t="shared" si="3"/>
+        <v>1.0647000000000001E-13</v>
       </c>
       <c r="Y51" s="32">
-        <f>L51*1000</f>
-        <v>15.964661286906612</v>
+        <f t="shared" si="3"/>
+        <v>30.108791023551941</v>
       </c>
       <c r="Z51" s="32">
-        <f>M51*1000</f>
-        <v>0.53495619399985317</v>
+        <f t="shared" si="3"/>
+        <v>0.63718604259144807</v>
       </c>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A52" s="12">
+        <v>200</v>
+      </c>
+      <c r="B52" s="19">
+        <f>V33</f>
+        <v>2.7399999999999999E-13</v>
+      </c>
+      <c r="C52" s="29">
+        <f>W33</f>
+        <v>1.5800000000000003E-14</v>
+      </c>
+      <c r="D52" s="19">
+        <f>V39</f>
+        <v>2.3246787487951729E-2</v>
+      </c>
+      <c r="E52" s="29">
+        <f>W39</f>
+        <v>5.8957214050769154E-4</v>
+      </c>
+      <c r="F52" s="19">
+        <f>V26</f>
+        <v>5.9040000000000006E-14</v>
+      </c>
+      <c r="G52" s="29">
+        <f>W26</f>
+        <v>4.3871200000000002E-16</v>
+      </c>
+      <c r="H52" s="19">
+        <f>V27</f>
+        <v>1.680490661779643E-2</v>
+      </c>
+      <c r="I52" s="29">
+        <f>W27</f>
+        <v>6.8339953579038819E-4</v>
+      </c>
+      <c r="J52" s="19">
+        <f>X26</f>
+        <v>6.8628000000000001E-14</v>
+      </c>
+      <c r="K52" s="19">
+        <f>Y26</f>
+        <v>2.4104200000000005E-16</v>
+      </c>
+      <c r="L52" s="19">
+        <f>X27</f>
+        <v>1.5964661286906611E-2</v>
+      </c>
+      <c r="M52" s="19">
+        <f>Y27</f>
+        <v>5.3495619399985313E-4</v>
+      </c>
+      <c r="N52" s="14">
+        <v>200</v>
+      </c>
+      <c r="O52" s="30">
+        <f t="shared" si="3"/>
+        <v>2.7399999999999998E-10</v>
+      </c>
+      <c r="P52" s="30">
+        <f t="shared" si="3"/>
+        <v>1.5800000000000003E-11</v>
+      </c>
+      <c r="Q52" s="32">
+        <f t="shared" si="3"/>
+        <v>23.246787487951728</v>
+      </c>
+      <c r="R52" s="32">
+        <f t="shared" si="3"/>
+        <v>0.58957214050769158</v>
+      </c>
+      <c r="S52" s="25">
+        <f t="shared" si="3"/>
+        <v>5.904000000000001E-11</v>
+      </c>
+      <c r="T52" s="25">
+        <f t="shared" si="3"/>
+        <v>4.38712E-13</v>
+      </c>
+      <c r="U52" s="32">
+        <f t="shared" si="3"/>
+        <v>16.80490661779643</v>
+      </c>
+      <c r="V52" s="32">
+        <f t="shared" si="3"/>
+        <v>0.68339953579038815</v>
+      </c>
+      <c r="W52" s="25">
+        <f t="shared" si="3"/>
+        <v>6.8627999999999996E-11</v>
+      </c>
+      <c r="X52" s="25">
+        <f t="shared" si="3"/>
+        <v>2.4104200000000004E-13</v>
+      </c>
+      <c r="Y52" s="32">
+        <f t="shared" si="3"/>
+        <v>15.964661286906612</v>
+      </c>
+      <c r="Z52" s="32">
+        <f t="shared" si="3"/>
+        <v>0.53495619399985317</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A53" s="12">
         <v>450</v>
       </c>
-      <c r="B52" s="19">
-        <f>Z32</f>
-        <v>2.0800000000000001E-4</v>
-      </c>
-      <c r="C52" s="29">
-        <f>AA32</f>
-        <v>6.5799999999999997E-6</v>
-      </c>
-      <c r="D52" s="19">
-        <f>Z38</f>
+      <c r="B53" s="19">
+        <f>Z33</f>
+        <v>2.0800000000000002E-13</v>
+      </c>
+      <c r="C53" s="29">
+        <f>AA33</f>
+        <v>6.5800000000000004E-15</v>
+      </c>
+      <c r="D53" s="19">
+        <f>Z39</f>
         <v>1.55445386214617E-2</v>
       </c>
-      <c r="E52" s="29">
-        <f>AA38</f>
+      <c r="E53" s="29">
+        <f>AA39</f>
         <v>8.0523510876941238E-4</v>
       </c>
-      <c r="F52" s="19">
-        <f>Z25</f>
-        <v>1.18306E-4</v>
-      </c>
-      <c r="G52" s="29">
-        <f>AA25</f>
-        <v>3.3899399999999998E-6</v>
-      </c>
-      <c r="H52" s="19">
+      <c r="F53" s="19">
         <f>Z26</f>
+        <v>1.1830600000000002E-13</v>
+      </c>
+      <c r="G53" s="29">
+        <f>AA26</f>
+        <v>3.38994E-15</v>
+      </c>
+      <c r="H53" s="19">
+        <f>Z27</f>
         <v>5.5596232727209861E-3</v>
       </c>
-      <c r="I52" s="29">
-        <f>AA26</f>
+      <c r="I53" s="29">
+        <f>AA27</f>
         <v>7.1280812237153196E-4</v>
       </c>
-      <c r="J52" s="19">
-        <f>AB25</f>
-        <v>1.17705E-4</v>
-      </c>
-      <c r="K52" s="19">
-        <f>AC25</f>
-        <v>1.21875E-6</v>
-      </c>
-      <c r="L52" s="19">
+      <c r="J53" s="19">
         <f>AB26</f>
+        <v>1.17705E-13</v>
+      </c>
+      <c r="K53" s="19">
+        <f>AC26</f>
+        <v>1.2187499999999999E-15</v>
+      </c>
+      <c r="L53" s="19">
+        <f>AB27</f>
         <v>5.5876314504173137E-3</v>
       </c>
-      <c r="M52" s="19">
-        <f>AC26</f>
+      <c r="M53" s="19">
+        <f>AC27</f>
         <v>4.5513288756532003E-4</v>
       </c>
-      <c r="N52" s="14">
+      <c r="N53" s="14">
         <v>450</v>
       </c>
-      <c r="O52" s="30">
-        <f>B52*1000</f>
-        <v>0.20800000000000002</v>
-      </c>
-      <c r="P52" s="30">
-        <f>C52*1000</f>
-        <v>6.5799999999999999E-3</v>
-      </c>
-      <c r="Q52" s="32">
-        <f>D52*1000</f>
+      <c r="O53" s="30">
+        <f t="shared" si="3"/>
+        <v>2.0800000000000003E-10</v>
+      </c>
+      <c r="P53" s="30">
+        <f t="shared" si="3"/>
+        <v>6.5800000000000006E-12</v>
+      </c>
+      <c r="Q53" s="32">
+        <f t="shared" si="3"/>
         <v>15.544538621461699</v>
       </c>
-      <c r="R52" s="32">
-        <f>E52*1000</f>
+      <c r="R53" s="32">
+        <f t="shared" si="3"/>
         <v>0.8052351087694124</v>
       </c>
-      <c r="S52" s="31">
-        <f>F52*1000</f>
-        <v>0.11830600000000001</v>
-      </c>
-      <c r="T52" s="31">
-        <f>G52*1000</f>
-        <v>3.3899399999999997E-3</v>
-      </c>
-      <c r="U52" s="32">
-        <f>H52*1000</f>
+      <c r="S53" s="31">
+        <f t="shared" si="3"/>
+        <v>1.1830600000000002E-10</v>
+      </c>
+      <c r="T53" s="31">
+        <f t="shared" si="3"/>
+        <v>3.38994E-12</v>
+      </c>
+      <c r="U53" s="32">
+        <f t="shared" si="3"/>
         <v>5.5596232727209864</v>
       </c>
-      <c r="V52" s="32">
-        <f>I52*1000</f>
+      <c r="V53" s="32">
+        <f t="shared" si="3"/>
         <v>0.7128081223715319</v>
       </c>
-      <c r="W52" s="31">
-        <f>J52*1000</f>
-        <v>0.117705</v>
-      </c>
-      <c r="X52" s="31">
-        <f>K52*1000</f>
-        <v>1.21875E-3</v>
-      </c>
-      <c r="Y52" s="32">
-        <f>L52*1000</f>
+      <c r="W53" s="31">
+        <f t="shared" si="3"/>
+        <v>1.1770500000000001E-10</v>
+      </c>
+      <c r="X53" s="31">
+        <f t="shared" si="3"/>
+        <v>1.21875E-12</v>
+      </c>
+      <c r="Y53" s="32">
+        <f t="shared" si="3"/>
         <v>5.5876314504173141</v>
       </c>
-      <c r="Z52" s="32">
-        <f>M52*1000</f>
+      <c r="Z53" s="32">
+        <f t="shared" si="3"/>
         <v>0.45513288756532005</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="W44:Z44"/>
-    <mergeCell ref="S44:V44"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="O44:P44"/>
-    <mergeCell ref="Q44:R44"/>
-    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="W45:Z45"/>
+    <mergeCell ref="S45:V45"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="O45:P45"/>
+    <mergeCell ref="Q45:R45"/>
+    <mergeCell ref="J45:M45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>